<commit_message>
Add RFE in feature selection
</commit_message>
<xml_diff>
--- a/results/recommendations.xlsx
+++ b/results/recommendations.xlsx
@@ -43,10 +43,10 @@
     <t>Best_Revenue</t>
   </si>
   <si>
-    <t>CL</t>
+    <t>CC</t>
   </si>
   <si>
-    <t>CC</t>
+    <t>CL</t>
   </si>
   <si>
     <t>MF</t>
@@ -444,147 +444,147 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B2">
-        <v>1.045295834541321</v>
+        <v>72.32727813720703</v>
       </c>
       <c r="C2">
-        <v>0.3310142457485199</v>
+        <v>0.3931759297847748</v>
       </c>
       <c r="D2">
-        <v>27.81558799743652</v>
+        <v>1.174347400665283</v>
       </c>
       <c r="E2">
-        <v>0.7662035822868347</v>
+        <v>0.4449374973773956</v>
       </c>
       <c r="F2">
-        <v>0.3502905964851379</v>
+        <v>0.3367405235767365</v>
       </c>
       <c r="G2">
-        <v>0.6278699040412903</v>
+        <v>0.2501336932182312</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
       </c>
       <c r="I2">
-        <v>27.81558799743652</v>
+        <v>72.32727813720703</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>0.365460216999054</v>
+        <v>53.65043640136719</v>
       </c>
       <c r="C3">
-        <v>0.4977242946624756</v>
+        <v>0.3969834446907043</v>
       </c>
       <c r="D3">
-        <v>25.25651168823242</v>
+        <v>1.423470258712769</v>
       </c>
       <c r="E3">
-        <v>0.320733517408371</v>
+        <v>0.625212550163269</v>
       </c>
       <c r="F3">
-        <v>0.2755052745342255</v>
+        <v>0.5093652606010437</v>
       </c>
       <c r="G3">
-        <v>0.5721834301948547</v>
+        <v>0.6683977842330933</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>
       </c>
       <c r="I3">
-        <v>25.25651168823242</v>
+        <v>53.65043640136719</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>20.34809684753418</v>
+        <v>32.23302841186523</v>
       </c>
       <c r="C4">
-        <v>0.3494563102722168</v>
+        <v>0.2178645431995392</v>
       </c>
       <c r="D4">
-        <v>0.6382906436920166</v>
+        <v>1.396708488464355</v>
       </c>
       <c r="E4">
-        <v>0.5033221244812012</v>
+        <v>0.6679288148880005</v>
       </c>
       <c r="F4">
-        <v>0.383391410112381</v>
+        <v>0.2088626623153687</v>
       </c>
       <c r="G4">
-        <v>0.4460285902023315</v>
+        <v>0.4115189611911774</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I4">
-        <v>20.34809684753418</v>
+        <v>32.23302841186523</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B5">
-        <v>0.648482084274292</v>
+        <v>24.36797904968262</v>
       </c>
       <c r="C5">
-        <v>16.88318061828613</v>
+        <v>0.800474226474762</v>
       </c>
       <c r="D5">
-        <v>0.9237433075904846</v>
+        <v>1.760137557983398</v>
       </c>
       <c r="E5">
-        <v>0.4538939893245697</v>
+        <v>0.504950225353241</v>
       </c>
       <c r="F5">
-        <v>0.6331732869148254</v>
+        <v>0.6800346970558167</v>
       </c>
       <c r="G5">
-        <v>0.4465542733669281</v>
+        <v>0.3917422890663147</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I5">
-        <v>16.88318061828613</v>
+        <v>24.36797904968262</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>0.7631844282150269</v>
+        <v>23.42295074462891</v>
       </c>
       <c r="C6">
-        <v>0.2568281292915344</v>
+        <v>0.6047609448432922</v>
       </c>
       <c r="D6">
-        <v>12.57154369354248</v>
+        <v>0.4544323682785034</v>
       </c>
       <c r="E6">
-        <v>0.4801252484321594</v>
+        <v>0.485367476940155</v>
       </c>
       <c r="F6">
-        <v>0.2642067074775696</v>
+        <v>0.551078200340271</v>
       </c>
       <c r="G6">
-        <v>0.7658824920654297</v>
+        <v>0.2117873728275299</v>
       </c>
       <c r="H6" t="s">
         <v>9</v>
       </c>
       <c r="I6">
-        <v>12.57154369354248</v>
+        <v>23.42295074462891</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -592,173 +592,173 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>1.5652756690979</v>
+        <v>0.4489038586616516</v>
       </c>
       <c r="C7">
-        <v>0.256329357624054</v>
+        <v>0.291985422372818</v>
       </c>
       <c r="D7">
-        <v>11.97526741027832</v>
+        <v>13.98909187316895</v>
       </c>
       <c r="E7">
-        <v>0.4809494018554688</v>
+        <v>0.3867040872573853</v>
       </c>
       <c r="F7">
-        <v>0.2578696310520172</v>
+        <v>0.2270368933677673</v>
       </c>
       <c r="G7">
-        <v>0.7292747497558594</v>
+        <v>0.7905167937278748</v>
       </c>
       <c r="H7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I7">
-        <v>11.97526741027832</v>
+        <v>13.98909187316895</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>1.5652756690979</v>
+        <v>1.063194513320923</v>
       </c>
       <c r="C8">
-        <v>0.2270082086324692</v>
+        <v>0.5582491755485535</v>
       </c>
       <c r="D8">
-        <v>11.80993556976318</v>
+        <v>13.95850276947021</v>
       </c>
       <c r="E8">
-        <v>0.4809494018554688</v>
+        <v>0.7681990265846252</v>
       </c>
       <c r="F8">
-        <v>0.2335300892591476</v>
+        <v>0.4398095607757568</v>
       </c>
       <c r="G8">
-        <v>0.7432284355163574</v>
+        <v>0.2557952702045441</v>
       </c>
       <c r="H8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I8">
-        <v>11.80993556976318</v>
+        <v>13.95850276947021</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>0.2991992831230164</v>
+        <v>0.492353767156601</v>
       </c>
       <c r="C9">
-        <v>10.87616443634033</v>
+        <v>0.3013112246990204</v>
       </c>
       <c r="D9">
-        <v>0.8548833727836609</v>
+        <v>13.58257961273193</v>
       </c>
       <c r="E9">
-        <v>0.2719557881355286</v>
+        <v>0.3738916516304016</v>
       </c>
       <c r="F9">
-        <v>0.4078909754753113</v>
+        <v>0.3235803246498108</v>
       </c>
       <c r="G9">
-        <v>0.4368325769901276</v>
+        <v>0.7615388631820679</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I9">
-        <v>10.87616443634033</v>
+        <v>13.58257961273193</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>1.844174385070801</v>
+        <v>12.8204517364502</v>
       </c>
       <c r="C10">
-        <v>0.2246222794055939</v>
+        <v>0.3878532350063324</v>
       </c>
       <c r="D10">
-        <v>10.57874965667725</v>
+        <v>0.6051624417304993</v>
       </c>
       <c r="E10">
-        <v>0.7722392678260803</v>
+        <v>0.7900606989860535</v>
       </c>
       <c r="F10">
-        <v>0.268760621547699</v>
+        <v>0.2662014365196228</v>
       </c>
       <c r="G10">
-        <v>0.7293388247489929</v>
+        <v>0.2279759347438812</v>
       </c>
       <c r="H10" t="s">
         <v>9</v>
       </c>
       <c r="I10">
-        <v>10.57874965667725</v>
+        <v>12.8204517364502</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>0.4441219568252563</v>
+        <v>12.31007862091064</v>
       </c>
       <c r="C11">
-        <v>10.3818244934082</v>
+        <v>0.3864842355251312</v>
       </c>
       <c r="D11">
-        <v>0.9692776203155518</v>
+        <v>0.3260757923126221</v>
       </c>
       <c r="E11">
-        <v>0.3989695608615875</v>
+        <v>0.7586089372634888</v>
       </c>
       <c r="F11">
-        <v>0.3893516659736633</v>
+        <v>0.3500140607357025</v>
       </c>
       <c r="G11">
-        <v>0.5843170285224915</v>
+        <v>0.2345577031373978</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I11">
-        <v>10.3818244934082</v>
+        <v>12.31007862091064</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>0.6942785382270813</v>
+        <v>9.46833610534668</v>
       </c>
       <c r="C12">
-        <v>10.34127902984619</v>
+        <v>0.2600335776805878</v>
       </c>
       <c r="D12">
-        <v>2.138457775115967</v>
+        <v>0.6422207355499268</v>
       </c>
       <c r="E12">
-        <v>0.4462517499923706</v>
+        <v>0.5103054642677307</v>
       </c>
       <c r="F12">
-        <v>0.6824838519096375</v>
+        <v>0.2433930039405823</v>
       </c>
       <c r="G12">
-        <v>0.4089968800544739</v>
+        <v>0.2926400303840637</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I12">
-        <v>10.34127902984619</v>
+        <v>9.46833610534668</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -766,753 +766,753 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <v>0.7631844282150269</v>
+        <v>0.5113710165023804</v>
       </c>
       <c r="C13">
-        <v>0.173862487077713</v>
+        <v>0.2278967499732971</v>
       </c>
       <c r="D13">
-        <v>9.516219139099121</v>
+        <v>9.077680587768555</v>
       </c>
       <c r="E13">
-        <v>0.4801252484321594</v>
+        <v>0.4055269956588745</v>
       </c>
       <c r="F13">
-        <v>0.201418861746788</v>
+        <v>0.2447399944067001</v>
       </c>
       <c r="G13">
-        <v>0.6908400058746338</v>
+        <v>0.6707048416137695</v>
       </c>
       <c r="H13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I13">
-        <v>9.516219139099121</v>
+        <v>9.077680587768555</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B14">
-        <v>4.059774398803711</v>
+        <v>8.579387664794922</v>
       </c>
       <c r="C14">
-        <v>0.3236365616321564</v>
+        <v>0.3155757784843445</v>
       </c>
       <c r="D14">
-        <v>9.345794677734375</v>
+        <v>0.6188979148864746</v>
       </c>
       <c r="E14">
-        <v>0.4801252484321594</v>
+        <v>0.5287050008773804</v>
       </c>
       <c r="F14">
-        <v>0.2817999422550201</v>
+        <v>0.2049365341663361</v>
       </c>
       <c r="G14">
-        <v>0.7699369788169861</v>
+        <v>0.2948892712593079</v>
       </c>
       <c r="H14" t="s">
         <v>9</v>
       </c>
       <c r="I14">
-        <v>9.345794677734375</v>
+        <v>8.579387664794922</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>0.5150685906410217</v>
+        <v>1.013941764831543</v>
       </c>
       <c r="C15">
-        <v>0.9078059196472168</v>
+        <v>8.156551361083984</v>
       </c>
       <c r="D15">
-        <v>8.250652313232422</v>
+        <v>0.9895534515380859</v>
       </c>
       <c r="E15">
-        <v>0.3597941100597382</v>
+        <v>0.5048841834068298</v>
       </c>
       <c r="F15">
-        <v>0.4911316931247711</v>
+        <v>0.5306404232978821</v>
       </c>
       <c r="G15">
-        <v>0.6995679140090942</v>
+        <v>0.4500592648983002</v>
       </c>
       <c r="H15" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I15">
-        <v>8.250652313232422</v>
+        <v>8.156551361083984</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B16">
-        <v>0.5363700985908508</v>
+        <v>0.4722757935523987</v>
       </c>
       <c r="C16">
-        <v>1.704368829727173</v>
+        <v>0.6049237251281738</v>
       </c>
       <c r="D16">
-        <v>8.242794036865234</v>
+        <v>8.075596809387207</v>
       </c>
       <c r="E16">
-        <v>0.3177151679992676</v>
+        <v>0.3082205653190613</v>
       </c>
       <c r="F16">
-        <v>0.4328040778636932</v>
+        <v>0.6395595073699951</v>
       </c>
       <c r="G16">
-        <v>0.6700464487075806</v>
+        <v>0.7907135486602783</v>
       </c>
       <c r="H16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I16">
-        <v>8.242794036865234</v>
+        <v>8.075596809387207</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B17">
-        <v>1.048369646072388</v>
+        <v>7.924840927124023</v>
       </c>
       <c r="C17">
-        <v>7.897205352783203</v>
+        <v>0.2855639159679413</v>
       </c>
       <c r="D17">
-        <v>1.140721797943115</v>
+        <v>0.7000500559806824</v>
       </c>
       <c r="E17">
-        <v>0.531887412071228</v>
+        <v>0.4271172285079956</v>
       </c>
       <c r="F17">
-        <v>0.5622509717941284</v>
+        <v>0.2843851447105408</v>
       </c>
       <c r="G17">
-        <v>0.534702479839325</v>
+        <v>0.3179340660572052</v>
       </c>
       <c r="H17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I17">
-        <v>7.897205352783203</v>
+        <v>7.924840927124023</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B18">
-        <v>0.7631844282150269</v>
+        <v>0.4288828670978546</v>
       </c>
       <c r="C18">
-        <v>0.4417754113674164</v>
+        <v>7.879054546356201</v>
       </c>
       <c r="D18">
-        <v>7.723196983337402</v>
+        <v>0.6754574775695801</v>
       </c>
       <c r="E18">
-        <v>0.4801252484321594</v>
+        <v>0.2135587930679321</v>
       </c>
       <c r="F18">
-        <v>0.2726500630378723</v>
+        <v>0.3484592139720917</v>
       </c>
       <c r="G18">
-        <v>0.6290992498397827</v>
+        <v>0.4210911691188812</v>
       </c>
       <c r="H18" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I18">
-        <v>7.723196983337402</v>
+        <v>7.879054546356201</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19">
-        <v>0.5734889507293701</v>
+        <v>0.4235605001449585</v>
       </c>
       <c r="C19">
-        <v>0.4043719172477722</v>
+        <v>0.2657084167003632</v>
       </c>
       <c r="D19">
-        <v>7.711616516113281</v>
+        <v>7.855395793914795</v>
       </c>
       <c r="E19">
-        <v>0.4609253406524658</v>
+        <v>0.3216502964496613</v>
       </c>
       <c r="F19">
-        <v>0.4139429926872253</v>
+        <v>0.2725946307182312</v>
       </c>
       <c r="G19">
-        <v>0.7861724495887756</v>
+        <v>0.4887738823890686</v>
       </c>
       <c r="H19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I19">
-        <v>7.711616516113281</v>
+        <v>7.855395793914795</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B20">
-        <v>0.5363700985908508</v>
+        <v>0.8569344878196716</v>
       </c>
       <c r="C20">
-        <v>0.4393652677536011</v>
+        <v>0.2625806331634521</v>
       </c>
       <c r="D20">
-        <v>7.436180591583252</v>
+        <v>7.817061901092529</v>
       </c>
       <c r="E20">
-        <v>0.3177151679992676</v>
+        <v>0.5143541097640991</v>
       </c>
       <c r="F20">
-        <v>0.3870207369327545</v>
+        <v>0.3986643850803375</v>
       </c>
       <c r="G20">
-        <v>0.636302649974823</v>
+        <v>0.6889245510101318</v>
       </c>
       <c r="H20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I20">
-        <v>7.436180591583252</v>
+        <v>7.817061901092529</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B21">
-        <v>0.8696997761726379</v>
+        <v>0.6891282796859741</v>
       </c>
       <c r="C21">
-        <v>0.5037468671798706</v>
+        <v>0.2120774835348129</v>
       </c>
       <c r="D21">
-        <v>7.045658111572266</v>
+        <v>7.23508882522583</v>
       </c>
       <c r="E21">
-        <v>0.4656721949577332</v>
+        <v>0.4136325120925903</v>
       </c>
       <c r="F21">
-        <v>0.3455341160297394</v>
+        <v>0.2275406420230865</v>
       </c>
       <c r="G21">
-        <v>0.7748391032218933</v>
+        <v>0.7843341827392578</v>
       </c>
       <c r="H21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I21">
-        <v>7.045658111572266</v>
+        <v>7.23508882522583</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B22">
-        <v>1.458858132362366</v>
+        <v>0.8474979400634766</v>
       </c>
       <c r="C22">
-        <v>0.5653607249259949</v>
+        <v>0.4901507198810577</v>
       </c>
       <c r="D22">
-        <v>6.775723934173584</v>
+        <v>7.13730525970459</v>
       </c>
       <c r="E22">
-        <v>0.4470676779747009</v>
+        <v>0.4080877304077148</v>
       </c>
       <c r="F22">
-        <v>0.406427413225174</v>
+        <v>0.4433773756027222</v>
       </c>
       <c r="G22">
-        <v>0.6977027058601379</v>
+        <v>0.7709833383560181</v>
       </c>
       <c r="H22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I22">
-        <v>6.775723934173584</v>
+        <v>7.13730525970459</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23">
-        <v>0.6077439188957214</v>
+        <v>0.4259302020072937</v>
       </c>
       <c r="C23">
-        <v>0.4675746560096741</v>
+        <v>0.3195417821407318</v>
       </c>
       <c r="D23">
-        <v>6.722147941589355</v>
+        <v>6.989850521087646</v>
       </c>
       <c r="E23">
-        <v>0.4127833545207977</v>
+        <v>0.328326940536499</v>
       </c>
       <c r="F23">
-        <v>0.3615009486675262</v>
+        <v>0.3069196343421936</v>
       </c>
       <c r="G23">
-        <v>0.748699426651001</v>
+        <v>0.7950443029403687</v>
       </c>
       <c r="H23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I23">
-        <v>6.722147941589355</v>
+        <v>6.989850521087646</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B24">
-        <v>1.398959279060364</v>
+        <v>0.3423245549201965</v>
       </c>
       <c r="C24">
-        <v>0.2958044409751892</v>
+        <v>0.9769492149353027</v>
       </c>
       <c r="D24">
-        <v>6.707241535186768</v>
+        <v>6.500402927398682</v>
       </c>
       <c r="E24">
-        <v>0.4725532233715057</v>
+        <v>0.2742345333099365</v>
       </c>
       <c r="F24">
-        <v>0.2801662981510162</v>
+        <v>0.4473406076431274</v>
       </c>
       <c r="G24">
-        <v>0.7294818162918091</v>
+        <v>0.7764785885810852</v>
       </c>
       <c r="H24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I24">
-        <v>6.707241535186768</v>
+        <v>6.500402927398682</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B25">
-        <v>6.668867111206055</v>
+        <v>0.9134219288825989</v>
       </c>
       <c r="C25">
-        <v>0.4051163196563721</v>
+        <v>6.426394939422607</v>
       </c>
       <c r="D25">
-        <v>0.4988072216510773</v>
+        <v>0.8856394290924072</v>
       </c>
       <c r="E25">
-        <v>0.4265473484992981</v>
+        <v>0.6208049654960632</v>
       </c>
       <c r="F25">
-        <v>0.3565329313278198</v>
+        <v>0.5612607598304749</v>
       </c>
       <c r="G25">
-        <v>0.3607816696166992</v>
+        <v>0.437241792678833</v>
       </c>
       <c r="H25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I25">
-        <v>6.668867111206055</v>
+        <v>6.426394939422607</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B26">
-        <v>0.3581043183803558</v>
+        <v>0.4286714494228363</v>
       </c>
       <c r="C26">
-        <v>0.6211801767349243</v>
+        <v>0.6489058136940002</v>
       </c>
       <c r="D26">
-        <v>6.490583419799805</v>
+        <v>6.41123628616333</v>
       </c>
       <c r="E26">
-        <v>0.2642917335033417</v>
+        <v>0.3099444806575775</v>
       </c>
       <c r="F26">
-        <v>0.5104377865791321</v>
+        <v>0.3972028791904449</v>
       </c>
       <c r="G26">
-        <v>0.6650115847587585</v>
+        <v>0.7949239015579224</v>
       </c>
       <c r="H26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I26">
-        <v>6.490583419799805</v>
+        <v>6.41123628616333</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B27">
-        <v>1.458858132362366</v>
+        <v>4.518557548522949</v>
       </c>
       <c r="C27">
-        <v>6.36452054977417</v>
+        <v>1.022661924362183</v>
       </c>
       <c r="D27">
-        <v>1.838299512863159</v>
+        <v>6.39005184173584</v>
       </c>
       <c r="E27">
-        <v>0.4470676779747009</v>
+        <v>0.2781537175178528</v>
       </c>
       <c r="F27">
-        <v>0.5733299255371094</v>
+        <v>0.4067932367324829</v>
       </c>
       <c r="G27">
-        <v>0.5132831335067749</v>
+        <v>0.771868109703064</v>
       </c>
       <c r="H27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I27">
-        <v>6.36452054977417</v>
+        <v>6.39005184173584</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B28">
-        <v>1.5652756690979</v>
+        <v>0.7308862805366516</v>
       </c>
       <c r="C28">
-        <v>0.2982769906520844</v>
+        <v>0.4886845350265503</v>
       </c>
       <c r="D28">
-        <v>6.142238616943359</v>
+        <v>6.272773742675781</v>
       </c>
       <c r="E28">
-        <v>0.4809494018554688</v>
+        <v>0.3519368171691895</v>
       </c>
       <c r="F28">
-        <v>0.3371121287345886</v>
+        <v>0.4280272424221039</v>
       </c>
       <c r="G28">
-        <v>0.7157319188117981</v>
+        <v>0.7160928845405579</v>
       </c>
       <c r="H28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I28">
-        <v>6.142238616943359</v>
+        <v>6.272773742675781</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B29">
-        <v>0.9573426246643066</v>
+        <v>3.351975917816162</v>
       </c>
       <c r="C29">
-        <v>0.3661803603172302</v>
+        <v>0.9243535995483398</v>
       </c>
       <c r="D29">
-        <v>5.790181636810303</v>
+        <v>6.234553337097168</v>
       </c>
       <c r="E29">
-        <v>0.4875599145889282</v>
+        <v>0.3920775055885315</v>
       </c>
       <c r="F29">
-        <v>0.4152425229549408</v>
+        <v>0.4871386289596558</v>
       </c>
       <c r="G29">
-        <v>0.6773995757102966</v>
+        <v>0.792801558971405</v>
       </c>
       <c r="H29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I29">
-        <v>5.790181636810303</v>
+        <v>6.234553337097168</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B30">
-        <v>5.448350429534912</v>
+        <v>0.6135110855102539</v>
       </c>
       <c r="C30">
-        <v>0.6786563992500305</v>
+        <v>0.7021892070770264</v>
       </c>
       <c r="D30">
-        <v>5.779759407043457</v>
+        <v>6.010499954223633</v>
       </c>
       <c r="E30">
-        <v>0.6577000617980957</v>
+        <v>0.4375878572463989</v>
       </c>
       <c r="F30">
-        <v>0.3496769368648529</v>
+        <v>0.5093652606010437</v>
       </c>
       <c r="G30">
-        <v>0.6925519704818726</v>
+        <v>0.6640572547912598</v>
       </c>
       <c r="H30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I30">
-        <v>5.779759407043457</v>
+        <v>6.010499954223633</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B31">
-        <v>0.5363700985908508</v>
+        <v>0.5407677888870239</v>
       </c>
       <c r="C31">
-        <v>5.677998065948486</v>
+        <v>0.5786744356155396</v>
       </c>
       <c r="D31">
-        <v>0.8390836119651794</v>
+        <v>5.961269378662109</v>
       </c>
       <c r="E31">
-        <v>0.3177151679992676</v>
+        <v>0.3729904890060425</v>
       </c>
       <c r="F31">
-        <v>0.3805296123027802</v>
+        <v>0.5064505338668823</v>
       </c>
       <c r="G31">
-        <v>0.4399675130844116</v>
+        <v>0.5512764453887939</v>
       </c>
       <c r="H31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I31">
-        <v>5.677998065948486</v>
+        <v>5.961269378662109</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B32">
-        <v>0.6520236134529114</v>
+        <v>0.5723186731338501</v>
       </c>
       <c r="C32">
-        <v>5.604222774505615</v>
+        <v>0.2942241132259369</v>
       </c>
       <c r="D32">
-        <v>1.480185151100159</v>
+        <v>5.89526891708374</v>
       </c>
       <c r="E32">
-        <v>0.4588369727134705</v>
+        <v>0.4138064682483673</v>
       </c>
       <c r="F32">
-        <v>0.5868245363235474</v>
+        <v>0.2379521727561951</v>
       </c>
       <c r="G32">
-        <v>0.4520525932312012</v>
+        <v>0.7934637069702148</v>
       </c>
       <c r="H32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I32">
-        <v>5.604222774505615</v>
+        <v>5.89526891708374</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B33">
-        <v>0.7631844282150269</v>
+        <v>1.42775297164917</v>
       </c>
       <c r="C33">
-        <v>5.574575424194336</v>
+        <v>0.2904433310031891</v>
       </c>
       <c r="D33">
-        <v>2.102447271347046</v>
+        <v>5.678623199462891</v>
       </c>
       <c r="E33">
-        <v>0.4801252484321594</v>
+        <v>0.5628227591514587</v>
       </c>
       <c r="F33">
-        <v>0.4120056331157684</v>
+        <v>0.2187499701976776</v>
       </c>
       <c r="G33">
-        <v>0.6614825129508972</v>
+        <v>0.616786003112793</v>
       </c>
       <c r="H33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I33">
-        <v>5.574575424194336</v>
+        <v>5.678623199462891</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B34">
-        <v>0.8297740817070007</v>
+        <v>0.4741286337375641</v>
       </c>
       <c r="C34">
-        <v>0.5159294605255127</v>
+        <v>0.2034213691949844</v>
       </c>
       <c r="D34">
-        <v>5.561302661895752</v>
+        <v>5.659033298492432</v>
       </c>
       <c r="E34">
-        <v>0.4462517499923706</v>
+        <v>0.3426439464092255</v>
       </c>
       <c r="F34">
-        <v>0.4482416212558746</v>
+        <v>0.2184557020664215</v>
       </c>
       <c r="G34">
-        <v>0.692320704460144</v>
+        <v>0.3497738838195801</v>
       </c>
       <c r="H34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I34">
-        <v>5.561302661895752</v>
+        <v>5.659033298492432</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B35">
-        <v>0.7217172384262085</v>
+        <v>0.4724365472793579</v>
       </c>
       <c r="C35">
-        <v>0.2461574524641037</v>
+        <v>0.5082722306251526</v>
       </c>
       <c r="D35">
-        <v>5.255506038665771</v>
+        <v>5.528110504150391</v>
       </c>
       <c r="E35">
-        <v>0.4364781081676483</v>
+        <v>0.2475945949554443</v>
       </c>
       <c r="F35">
-        <v>0.2314262390136719</v>
+        <v>0.309226006269455</v>
       </c>
       <c r="G35">
-        <v>0.6115179061889648</v>
+        <v>0.5096895694732666</v>
       </c>
       <c r="H35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I35">
-        <v>5.255506038665771</v>
+        <v>5.528110504150391</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B36">
-        <v>1.458858132362366</v>
+        <v>0.5826843976974487</v>
       </c>
       <c r="C36">
-        <v>5.176161766052246</v>
+        <v>0.276839941740036</v>
       </c>
       <c r="D36">
-        <v>0.8557661771774292</v>
+        <v>5.474831581115723</v>
       </c>
       <c r="E36">
-        <v>0.4470676779747009</v>
+        <v>0.4436034560203552</v>
       </c>
       <c r="F36">
-        <v>0.5401549935340881</v>
+        <v>0.2909498810768127</v>
       </c>
       <c r="G36">
-        <v>0.4056196212768555</v>
+        <v>0.6266071200370789</v>
       </c>
       <c r="H36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I36">
-        <v>5.176161766052246</v>
+        <v>5.474831581115723</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B37">
-        <v>1.458858132362366</v>
+        <v>0.7513706684112549</v>
       </c>
       <c r="C37">
-        <v>5.176161766052246</v>
+        <v>0.4133648872375488</v>
       </c>
       <c r="D37">
-        <v>1.271335005760193</v>
+        <v>5.345963478088379</v>
       </c>
       <c r="E37">
-        <v>0.4470676779747009</v>
+        <v>0.4678671956062317</v>
       </c>
       <c r="F37">
-        <v>0.5401549935340881</v>
+        <v>0.3243132531642914</v>
       </c>
       <c r="G37">
-        <v>0.4807198643684387</v>
+        <v>0.7790641188621521</v>
       </c>
       <c r="H37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I37">
-        <v>5.176161766052246</v>
+        <v>5.345963478088379</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B38">
-        <v>0.5363700985908508</v>
+        <v>0.477464884519577</v>
       </c>
       <c r="C38">
-        <v>1.143130779266357</v>
+        <v>0.3393128514289856</v>
       </c>
       <c r="D38">
-        <v>5.140010833740234</v>
+        <v>5.32615852355957</v>
       </c>
       <c r="E38">
-        <v>0.3177151679992676</v>
+        <v>0.3625850975513458</v>
       </c>
       <c r="F38">
-        <v>0.3653046786785126</v>
+        <v>0.3104285597801208</v>
       </c>
       <c r="G38">
-        <v>0.3849086463451385</v>
+        <v>0.7024275064468384</v>
       </c>
       <c r="H38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I38">
-        <v>5.140010833740234</v>
+        <v>5.32615852355957</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1520,492 +1520,492 @@
         <v>2</v>
       </c>
       <c r="B39">
-        <v>1.653002381324768</v>
+        <v>1.231008648872375</v>
       </c>
       <c r="C39">
-        <v>0.2669430673122406</v>
+        <v>0.4923030138015747</v>
       </c>
       <c r="D39">
-        <v>5.128311634063721</v>
+        <v>5.163406848907471</v>
       </c>
       <c r="E39">
-        <v>0.482860267162323</v>
+        <v>0.4231030941009521</v>
       </c>
       <c r="F39">
-        <v>0.2883613109588623</v>
+        <v>0.2708915174007416</v>
       </c>
       <c r="G39">
-        <v>0.7730064392089844</v>
+        <v>0.4638983011245728</v>
       </c>
       <c r="H39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I39">
-        <v>5.128311634063721</v>
+        <v>5.163406848907471</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B40">
-        <v>5.079705238342285</v>
+        <v>0.3245489597320557</v>
       </c>
       <c r="C40">
-        <v>0.915865421295166</v>
+        <v>0.2872713804244995</v>
       </c>
       <c r="D40">
-        <v>0.5348434448242188</v>
+        <v>5.117724895477295</v>
       </c>
       <c r="E40">
-        <v>0.5979554653167725</v>
+        <v>0.2352232336997986</v>
       </c>
       <c r="F40">
-        <v>0.4914565086364746</v>
+        <v>0.2174950242042542</v>
       </c>
       <c r="G40">
-        <v>0.27218097448349</v>
+        <v>0.7615388631820679</v>
       </c>
       <c r="H40" t="s">
         <v>10</v>
       </c>
       <c r="I40">
-        <v>5.079705238342285</v>
+        <v>5.117724895477295</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B41">
-        <v>1.867653012275696</v>
+        <v>5.069324493408203</v>
       </c>
       <c r="C41">
-        <v>1.703729152679443</v>
+        <v>0.3780682682991028</v>
       </c>
       <c r="D41">
-        <v>5.020196914672852</v>
+        <v>2.497116088867188</v>
       </c>
       <c r="E41">
-        <v>0.5130324959754944</v>
+        <v>0.3120578825473785</v>
       </c>
       <c r="F41">
-        <v>0.4807019829750061</v>
+        <v>0.3004328608512878</v>
       </c>
       <c r="G41">
-        <v>0.5618929862976074</v>
+        <v>0.7701890468597412</v>
       </c>
       <c r="H41" t="s">
         <v>9</v>
       </c>
       <c r="I41">
-        <v>5.020196914672852</v>
+        <v>5.069324493408203</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B42">
-        <v>1.458858132362366</v>
+        <v>0.6439355611801147</v>
       </c>
       <c r="C42">
-        <v>1.064763784408569</v>
+        <v>0.6781551241874695</v>
       </c>
       <c r="D42">
-        <v>4.985651969909668</v>
+        <v>5.00117301940918</v>
       </c>
       <c r="E42">
-        <v>0.4470676779747009</v>
+        <v>0.4600559175014496</v>
       </c>
       <c r="F42">
-        <v>0.434250146150589</v>
+        <v>0.3837210834026337</v>
       </c>
       <c r="G42">
-        <v>0.4378305673599243</v>
+        <v>0.7934637069702148</v>
       </c>
       <c r="H42" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I42">
-        <v>4.985651969909668</v>
+        <v>5.00117301940918</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B43">
-        <v>0.5063862204551697</v>
+        <v>0.2785486280918121</v>
       </c>
       <c r="C43">
-        <v>0.740118682384491</v>
+        <v>0.2701749503612518</v>
       </c>
       <c r="D43">
-        <v>4.979002475738525</v>
+        <v>5.00107479095459</v>
       </c>
       <c r="E43">
-        <v>0.2693254351615906</v>
+        <v>0.227186307311058</v>
       </c>
       <c r="F43">
-        <v>0.5350095629692078</v>
+        <v>0.2877107560634613</v>
       </c>
       <c r="G43">
-        <v>0.7455480098724365</v>
+        <v>0.7937372326850891</v>
       </c>
       <c r="H43" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I43">
-        <v>4.979002475738525</v>
+        <v>5.00107479095459</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="B44">
-        <v>1.458858132362366</v>
+        <v>0.4069178104400635</v>
       </c>
       <c r="C44">
-        <v>4.972604274749756</v>
+        <v>1.08289909362793</v>
       </c>
       <c r="D44">
-        <v>1.020147442817688</v>
+        <v>4.974560260772705</v>
       </c>
       <c r="E44">
-        <v>0.4470676779747009</v>
+        <v>0.263069212436676</v>
       </c>
       <c r="F44">
-        <v>0.4479430615901947</v>
+        <v>0.5266286730766296</v>
       </c>
       <c r="G44">
-        <v>0.5161828398704529</v>
+        <v>0.6561864614486694</v>
       </c>
       <c r="H44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I44">
-        <v>4.972604274749756</v>
+        <v>4.974560260772705</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B45">
-        <v>4.059774398803711</v>
+        <v>1.354509115219116</v>
       </c>
       <c r="C45">
-        <v>0.6217958927154541</v>
+        <v>0.3035514950752258</v>
       </c>
       <c r="D45">
-        <v>4.958730220794678</v>
+        <v>4.831519603729248</v>
       </c>
       <c r="E45">
-        <v>0.4801252484321594</v>
+        <v>0.4655507504940033</v>
       </c>
       <c r="F45">
-        <v>0.39344322681427</v>
+        <v>0.3010125458240509</v>
       </c>
       <c r="G45">
-        <v>0.7578147649765015</v>
+        <v>0.6119588017463684</v>
       </c>
       <c r="H45" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I45">
-        <v>4.958730220794678</v>
+        <v>4.831519603729248</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B46">
-        <v>0.7631844282150269</v>
+        <v>0.6395937204360962</v>
       </c>
       <c r="C46">
-        <v>0.2509884238243103</v>
+        <v>4.714669704437256</v>
       </c>
       <c r="D46">
-        <v>4.79094123840332</v>
+        <v>1.163462042808533</v>
       </c>
       <c r="E46">
-        <v>0.4801252484321594</v>
+        <v>0.4248944520950317</v>
       </c>
       <c r="F46">
-        <v>0.2844588756561279</v>
+        <v>0.5023835301399231</v>
       </c>
       <c r="G46">
-        <v>0.4880091547966003</v>
+        <v>0.4068045020103455</v>
       </c>
       <c r="H46" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I46">
-        <v>4.79094123840332</v>
+        <v>4.714669704437256</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="B47">
-        <v>1.5652756690979</v>
+        <v>4.01276683807373</v>
       </c>
       <c r="C47">
-        <v>0.2297073602676392</v>
+        <v>0.7633211612701416</v>
       </c>
       <c r="D47">
-        <v>4.692739009857178</v>
+        <v>4.614940643310547</v>
       </c>
       <c r="E47">
-        <v>0.4809494018554688</v>
+        <v>0.7574900984764099</v>
       </c>
       <c r="F47">
-        <v>0.2836259603500366</v>
+        <v>0.7204834818840027</v>
       </c>
       <c r="G47">
-        <v>0.5599477887153625</v>
+        <v>0.5914685130119324</v>
       </c>
       <c r="H47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I47">
-        <v>4.692739009857178</v>
+        <v>4.614940643310547</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B48">
-        <v>0.5908888578414917</v>
+        <v>0.4454178512096405</v>
       </c>
       <c r="C48">
-        <v>0.3818592429161072</v>
+        <v>0.6496652960777283</v>
       </c>
       <c r="D48">
-        <v>4.690825462341309</v>
+        <v>4.502804279327393</v>
       </c>
       <c r="E48">
-        <v>0.3104280233383179</v>
+        <v>0.2845769822597504</v>
       </c>
       <c r="F48">
-        <v>0.4322957694530487</v>
+        <v>0.38226318359375</v>
       </c>
       <c r="G48">
-        <v>0.4306975305080414</v>
+        <v>0.7945255041122437</v>
       </c>
       <c r="H48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I48">
-        <v>4.690825462341309</v>
+        <v>4.502804279327393</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B49">
-        <v>0.8297740817070007</v>
+        <v>4.500415802001953</v>
       </c>
       <c r="C49">
-        <v>0.3708389103412628</v>
+        <v>0.5569881796836853</v>
       </c>
       <c r="D49">
-        <v>4.669229507446289</v>
+        <v>4.179859161376953</v>
       </c>
       <c r="E49">
-        <v>0.4462517499923706</v>
+        <v>0.5264094471931458</v>
       </c>
       <c r="F49">
-        <v>0.4329047203063965</v>
+        <v>0.4748590886592865</v>
       </c>
       <c r="G49">
-        <v>0.5402871966362</v>
+        <v>0.39176145195961</v>
       </c>
       <c r="H49" t="s">
         <v>9</v>
       </c>
       <c r="I49">
-        <v>4.669229507446289</v>
+        <v>4.500415802001953</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B50">
-        <v>0.8316347002983093</v>
+        <v>0.5741632580757141</v>
       </c>
       <c r="C50">
-        <v>4.648855209350586</v>
+        <v>0.2683936953544617</v>
       </c>
       <c r="D50">
-        <v>1.406261205673218</v>
+        <v>4.430737018585205</v>
       </c>
       <c r="E50">
-        <v>0.4801252484321594</v>
+        <v>0.3272684216499329</v>
       </c>
       <c r="F50">
-        <v>0.3309808075428009</v>
+        <v>0.226508617401123</v>
       </c>
       <c r="G50">
-        <v>0.5486490726470947</v>
+        <v>0.7038629055023193</v>
       </c>
       <c r="H50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I50">
-        <v>4.648855209350586</v>
+        <v>4.430737018585205</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B51">
-        <v>0.6389287710189819</v>
+        <v>1.305639743804932</v>
       </c>
       <c r="C51">
-        <v>0.4246689677238464</v>
+        <v>4.369619846343994</v>
       </c>
       <c r="D51">
-        <v>4.508520603179932</v>
+        <v>0.7050962448120117</v>
       </c>
       <c r="E51">
-        <v>0.4125660359859467</v>
+        <v>0.3916561901569366</v>
       </c>
       <c r="F51">
-        <v>0.3345444202423096</v>
+        <v>0.5394195914268494</v>
       </c>
       <c r="G51">
-        <v>0.7258387804031372</v>
+        <v>0.3490701615810394</v>
       </c>
       <c r="H51" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I51">
-        <v>4.508520603179932</v>
+        <v>4.369619846343994</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B52">
-        <v>1.5652756690979</v>
+        <v>0.6664578914642334</v>
       </c>
       <c r="C52">
-        <v>0.6497772932052612</v>
+        <v>0.2978371977806091</v>
       </c>
       <c r="D52">
-        <v>4.341734886169434</v>
+        <v>4.332044124603271</v>
       </c>
       <c r="E52">
-        <v>0.4809494018554688</v>
+        <v>0.4753522574901581</v>
       </c>
       <c r="F52">
-        <v>0.4388987123966217</v>
+        <v>0.2598100900650024</v>
       </c>
       <c r="G52">
-        <v>0.6673853397369385</v>
+        <v>0.6294780969619751</v>
       </c>
       <c r="H52" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I52">
-        <v>4.341734886169434</v>
+        <v>4.332044124603271</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B53">
-        <v>0.6617484092712402</v>
+        <v>1.355974316596985</v>
       </c>
       <c r="C53">
-        <v>0.4671551287174225</v>
+        <v>4.268353939056396</v>
       </c>
       <c r="D53">
-        <v>4.260557174682617</v>
+        <v>1.982340812683105</v>
       </c>
       <c r="E53">
-        <v>0.4074892401695251</v>
+        <v>0.5961111783981323</v>
       </c>
       <c r="F53">
-        <v>0.4082011580467224</v>
+        <v>0.4303293526172638</v>
       </c>
       <c r="G53">
-        <v>0.6107251644134521</v>
+        <v>0.4786726534366608</v>
       </c>
       <c r="H53" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I53">
-        <v>4.260557174682617</v>
+        <v>4.268353939056396</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B54">
-        <v>2.051961660385132</v>
+        <v>0.6040122509002686</v>
       </c>
       <c r="C54">
-        <v>1.053532123565674</v>
+        <v>4.232094287872314</v>
       </c>
       <c r="D54">
-        <v>4.146805286407471</v>
+        <v>1.019957304000854</v>
       </c>
       <c r="E54">
-        <v>0.5558948516845703</v>
+        <v>0.3886113464832306</v>
       </c>
       <c r="F54">
-        <v>0.4155782461166382</v>
+        <v>0.5056653618812561</v>
       </c>
       <c r="G54">
-        <v>0.72230464220047</v>
+        <v>0.5104163885116577</v>
       </c>
       <c r="H54" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I54">
-        <v>4.146805286407471</v>
+        <v>4.232094287872314</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="B55">
-        <v>0.3703398704528809</v>
+        <v>0.580802857875824</v>
       </c>
       <c r="C55">
-        <v>0.439457505941391</v>
+        <v>0.2405484765768051</v>
       </c>
       <c r="D55">
-        <v>4.127371311187744</v>
+        <v>4.226453304290771</v>
       </c>
       <c r="E55">
-        <v>0.2669812738895416</v>
+        <v>0.413757711648941</v>
       </c>
       <c r="F55">
-        <v>0.3087621331214905</v>
+        <v>0.3130834102630615</v>
       </c>
       <c r="G55">
-        <v>0.525839626789093</v>
+        <v>0.5770449042320251</v>
       </c>
       <c r="H55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I55">
-        <v>4.127371311187744</v>
+        <v>4.226453304290771</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2013,57 +2013,57 @@
         <v>4</v>
       </c>
       <c r="B56">
-        <v>0.3947072923183441</v>
+        <v>1.409974813461304</v>
       </c>
       <c r="C56">
-        <v>0.6123867034912109</v>
+        <v>0.3102516233921051</v>
       </c>
       <c r="D56">
-        <v>4.10554313659668</v>
+        <v>4.214303493499756</v>
       </c>
       <c r="E56">
-        <v>0.3540250360965729</v>
+        <v>0.4725889563560486</v>
       </c>
       <c r="F56">
-        <v>0.4671696126461029</v>
+        <v>0.2924222946166992</v>
       </c>
       <c r="G56">
-        <v>0.7462085485458374</v>
+        <v>0.792801558971405</v>
       </c>
       <c r="H56" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I56">
-        <v>4.10554313659668</v>
+        <v>4.214303493499756</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B57">
-        <v>4.059774398803711</v>
+        <v>0.9113236665725708</v>
       </c>
       <c r="C57">
-        <v>0.3313524127006531</v>
+        <v>0.2839363515377045</v>
       </c>
       <c r="D57">
-        <v>0.6090028882026672</v>
+        <v>4.210516929626465</v>
       </c>
       <c r="E57">
-        <v>0.4801252484321594</v>
+        <v>0.2400173991918564</v>
       </c>
       <c r="F57">
-        <v>0.3423287868499756</v>
+        <v>0.3110118210315704</v>
       </c>
       <c r="G57">
-        <v>0.4023275077342987</v>
+        <v>0.4633802473545074</v>
       </c>
       <c r="H57" t="s">
         <v>10</v>
       </c>
       <c r="I57">
-        <v>4.059774398803711</v>
+        <v>4.210516929626465</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2071,144 +2071,144 @@
         <v>3</v>
       </c>
       <c r="B58">
-        <v>4.059774398803711</v>
+        <v>1.280049324035645</v>
       </c>
       <c r="C58">
-        <v>0.4949878454208374</v>
+        <v>0.4687378704547882</v>
       </c>
       <c r="D58">
-        <v>0.4518698751926422</v>
+        <v>4.209689617156982</v>
       </c>
       <c r="E58">
-        <v>0.4801252484321594</v>
+        <v>0.4944873452186584</v>
       </c>
       <c r="F58">
-        <v>0.4950961470603943</v>
+        <v>0.4602119922637939</v>
       </c>
       <c r="G58">
-        <v>0.3237633407115936</v>
+        <v>0.48182013630867</v>
       </c>
       <c r="H58" t="s">
         <v>10</v>
       </c>
       <c r="I58">
-        <v>4.059774398803711</v>
+        <v>4.209689617156982</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B59">
-        <v>4.059774398803711</v>
+        <v>4.18530797958374</v>
       </c>
       <c r="C59">
-        <v>0.3036167919635773</v>
+        <v>0.7246070504188538</v>
       </c>
       <c r="D59">
-        <v>1.030104517936707</v>
+        <v>0.3946442008018494</v>
       </c>
       <c r="E59">
-        <v>0.4801252484321594</v>
+        <v>0.7900606989860535</v>
       </c>
       <c r="F59">
-        <v>0.3527809977531433</v>
+        <v>0.6767404675483704</v>
       </c>
       <c r="G59">
-        <v>0.6295127868652344</v>
+        <v>0.2838813364505768</v>
       </c>
       <c r="H59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I59">
-        <v>4.059774398803711</v>
+        <v>4.18530797958374</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B60">
-        <v>4.059774398803711</v>
+        <v>0.6062703728675842</v>
       </c>
       <c r="C60">
-        <v>0.3976689279079437</v>
+        <v>0.3422911763191223</v>
       </c>
       <c r="D60">
-        <v>1.547436356544495</v>
+        <v>4.174132823944092</v>
       </c>
       <c r="E60">
-        <v>0.4801252484321594</v>
+        <v>0.3984362483024597</v>
       </c>
       <c r="F60">
-        <v>0.3924946784973145</v>
+        <v>0.3280433714389801</v>
       </c>
       <c r="G60">
-        <v>0.4582381248474121</v>
+        <v>0.3193092346191406</v>
       </c>
       <c r="H60" t="s">
         <v>10</v>
       </c>
       <c r="I60">
-        <v>4.059774398803711</v>
+        <v>4.174132823944092</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B61">
-        <v>4.059774398803711</v>
+        <v>0.3459592759609222</v>
       </c>
       <c r="C61">
-        <v>0.4860062301158905</v>
+        <v>4.143638134002686</v>
       </c>
       <c r="D61">
-        <v>0.3979384899139404</v>
+        <v>1.082437753677368</v>
       </c>
       <c r="E61">
-        <v>0.4801252484321594</v>
+        <v>0.2388529628515244</v>
       </c>
       <c r="F61">
-        <v>0.4158576130867004</v>
+        <v>0.4013699889183044</v>
       </c>
       <c r="G61">
-        <v>0.2802030742168427</v>
+        <v>0.4284962713718414</v>
       </c>
       <c r="H61" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I61">
-        <v>4.059774398803711</v>
+        <v>4.143638134002686</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B62">
-        <v>4.059774398803711</v>
+        <v>4.112292289733887</v>
       </c>
       <c r="C62">
-        <v>0.3169528543949127</v>
+        <v>2.036388397216797</v>
       </c>
       <c r="D62">
-        <v>1.207093715667725</v>
+        <v>3.237614870071411</v>
       </c>
       <c r="E62">
-        <v>0.4801252484321594</v>
+        <v>0.3712125718593597</v>
       </c>
       <c r="F62">
-        <v>0.409624308347702</v>
+        <v>0.4504758417606354</v>
       </c>
       <c r="G62">
-        <v>0.498313307762146</v>
+        <v>0.4522309005260468</v>
       </c>
       <c r="H62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I62">
-        <v>4.059774398803711</v>
+        <v>4.112292289733887</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2216,57 +2216,57 @@
         <v>2</v>
       </c>
       <c r="B63">
-        <v>4.059774398803711</v>
+        <v>3.367501974105835</v>
       </c>
       <c r="C63">
-        <v>0.4854547083377838</v>
+        <v>0.5562509894371033</v>
       </c>
       <c r="D63">
-        <v>1.921349763870239</v>
+        <v>3.883129119873047</v>
       </c>
       <c r="E63">
-        <v>0.4801252484321594</v>
+        <v>0.4338265061378479</v>
       </c>
       <c r="F63">
-        <v>0.3939917087554932</v>
+        <v>0.4865312278270721</v>
       </c>
       <c r="G63">
-        <v>0.6572543382644653</v>
+        <v>0.5591688752174377</v>
       </c>
       <c r="H63" t="s">
         <v>10</v>
       </c>
       <c r="I63">
-        <v>4.059774398803711</v>
+        <v>3.883129119873047</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B64">
-        <v>4.059774398803711</v>
+        <v>0.5188497304916382</v>
       </c>
       <c r="C64">
-        <v>0.9916781783103943</v>
+        <v>3.879443407058716</v>
       </c>
       <c r="D64">
-        <v>0.6306118369102478</v>
+        <v>3.853436708450317</v>
       </c>
       <c r="E64">
-        <v>0.4801252484321594</v>
+        <v>0.3600914776325226</v>
       </c>
       <c r="F64">
-        <v>0.6524130702018738</v>
+        <v>0.4543478488922119</v>
       </c>
       <c r="G64">
-        <v>0.3242023885250092</v>
+        <v>0.5509883761405945</v>
       </c>
       <c r="H64" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I64">
-        <v>4.059774398803711</v>
+        <v>3.879443407058716</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -2274,463 +2274,463 @@
         <v>2</v>
       </c>
       <c r="B65">
-        <v>4.059774398803711</v>
+        <v>0.7998548746109009</v>
       </c>
       <c r="C65">
-        <v>0.3470688164234161</v>
+        <v>2.511055469512939</v>
       </c>
       <c r="D65">
-        <v>0.8021699786186218</v>
+        <v>3.87824010848999</v>
       </c>
       <c r="E65">
-        <v>0.4801252484321594</v>
+        <v>0.591956615447998</v>
       </c>
       <c r="F65">
-        <v>0.2891518473625183</v>
+        <v>0.3666545152664185</v>
       </c>
       <c r="G65">
-        <v>0.4182242453098297</v>
+        <v>0.4530238807201385</v>
       </c>
       <c r="H65" t="s">
         <v>10</v>
       </c>
       <c r="I65">
-        <v>4.059774398803711</v>
+        <v>3.87824010848999</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B66">
-        <v>4.059774398803711</v>
+        <v>0.5584484338760376</v>
       </c>
       <c r="C66">
-        <v>1.444747805595398</v>
+        <v>0.6152045130729675</v>
       </c>
       <c r="D66">
-        <v>2.70336127281189</v>
+        <v>3.869146585464478</v>
       </c>
       <c r="E66">
-        <v>0.4801252484321594</v>
+        <v>0.272204726934433</v>
       </c>
       <c r="F66">
-        <v>0.6499410271644592</v>
+        <v>0.2968957722187042</v>
       </c>
       <c r="G66">
-        <v>0.4570022821426392</v>
+        <v>0.4179515242576599</v>
       </c>
       <c r="H66" t="s">
         <v>10</v>
       </c>
       <c r="I66">
-        <v>4.059774398803711</v>
+        <v>3.869146585464478</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B67">
-        <v>4.059774398803711</v>
+        <v>0.5153672695159912</v>
       </c>
       <c r="C67">
-        <v>1.255168557167053</v>
+        <v>1.450673818588257</v>
       </c>
       <c r="D67">
-        <v>0.3267861008644104</v>
+        <v>3.855592012405396</v>
       </c>
       <c r="E67">
-        <v>0.4801252484321594</v>
+        <v>0.3682010769844055</v>
       </c>
       <c r="F67">
-        <v>0.7106531262397766</v>
+        <v>0.6729082465171814</v>
       </c>
       <c r="G67">
-        <v>0.2283535748720169</v>
+        <v>0.4717908799648285</v>
       </c>
       <c r="H67" t="s">
         <v>10</v>
       </c>
       <c r="I67">
-        <v>4.059774398803711</v>
+        <v>3.855592012405396</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B68">
-        <v>4.059774398803711</v>
+        <v>1.044631600379944</v>
       </c>
       <c r="C68">
-        <v>0.3912400901317596</v>
+        <v>0.1993452161550522</v>
       </c>
       <c r="D68">
-        <v>0.9123934507369995</v>
+        <v>3.842098712921143</v>
       </c>
       <c r="E68">
-        <v>0.4801252484321594</v>
+        <v>0.7362015843391418</v>
       </c>
       <c r="F68">
-        <v>0.2796751856803894</v>
+        <v>0.2277786582708359</v>
       </c>
       <c r="G68">
-        <v>0.4910438358783722</v>
+        <v>0.5415493249893188</v>
       </c>
       <c r="H68" t="s">
         <v>10</v>
       </c>
       <c r="I68">
-        <v>4.059774398803711</v>
+        <v>3.842098712921143</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B69">
-        <v>4.059774398803711</v>
+        <v>0.4497923851013184</v>
       </c>
       <c r="C69">
-        <v>2.100473403930664</v>
+        <v>3.836776494979858</v>
       </c>
       <c r="D69">
-        <v>0.8168288469314575</v>
+        <v>1.168477535247803</v>
       </c>
       <c r="E69">
-        <v>0.4801252484321594</v>
+        <v>0.320427268743515</v>
       </c>
       <c r="F69">
-        <v>0.4577378332614899</v>
+        <v>0.585633397102356</v>
       </c>
       <c r="G69">
-        <v>0.3399332165718079</v>
+        <v>0.4303281009197235</v>
       </c>
       <c r="H69" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I69">
-        <v>4.059774398803711</v>
+        <v>3.836776494979858</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B70">
-        <v>4.059774398803711</v>
+        <v>0.582064151763916</v>
       </c>
       <c r="C70">
-        <v>0.3905957341194153</v>
+        <v>0.6740126609802246</v>
       </c>
       <c r="D70">
-        <v>1.26423704624176</v>
+        <v>3.787899971008301</v>
       </c>
       <c r="E70">
-        <v>0.4801252484321594</v>
+        <v>0.380597710609436</v>
       </c>
       <c r="F70">
-        <v>0.3254152238368988</v>
+        <v>0.3769183754920959</v>
       </c>
       <c r="G70">
-        <v>0.6007080674171448</v>
+        <v>0.681069552898407</v>
       </c>
       <c r="H70" t="s">
         <v>10</v>
       </c>
       <c r="I70">
-        <v>4.059774398803711</v>
+        <v>3.787899971008301</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B71">
-        <v>4.059774398803711</v>
+        <v>0.6732867956161499</v>
       </c>
       <c r="C71">
-        <v>0.2140310406684875</v>
+        <v>0.493439108133316</v>
       </c>
       <c r="D71">
-        <v>1.561733245849609</v>
+        <v>3.719396352767944</v>
       </c>
       <c r="E71">
-        <v>0.4801252484321594</v>
+        <v>0.4868099689483643</v>
       </c>
       <c r="F71">
-        <v>0.2725474238395691</v>
+        <v>0.415654718875885</v>
       </c>
       <c r="G71">
-        <v>0.4240571260452271</v>
+        <v>0.6389650702476501</v>
       </c>
       <c r="H71" t="s">
         <v>10</v>
       </c>
       <c r="I71">
-        <v>4.059774398803711</v>
+        <v>3.719396352767944</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B72">
-        <v>4.059774398803711</v>
+        <v>0.5916579365730286</v>
       </c>
       <c r="C72">
-        <v>0.39597287774086</v>
+        <v>0.1805351376533508</v>
       </c>
       <c r="D72">
-        <v>0.5471372008323669</v>
+        <v>3.696828126907349</v>
       </c>
       <c r="E72">
-        <v>0.4801252484321594</v>
+        <v>0.4547415375709534</v>
       </c>
       <c r="F72">
-        <v>0.3140995800495148</v>
+        <v>0.2643669247627258</v>
       </c>
       <c r="G72">
-        <v>0.3480830788612366</v>
+        <v>0.5296776294708252</v>
       </c>
       <c r="H72" t="s">
         <v>10</v>
       </c>
       <c r="I72">
-        <v>4.059774398803711</v>
+        <v>3.696828126907349</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B73">
-        <v>4.059774398803711</v>
+        <v>0.7457153797149658</v>
       </c>
       <c r="C73">
-        <v>1.59918737411499</v>
+        <v>0.3995901346206665</v>
       </c>
       <c r="D73">
-        <v>1.217051267623901</v>
+        <v>3.674150228500366</v>
       </c>
       <c r="E73">
-        <v>0.4801252484321594</v>
+        <v>0.4353805780410767</v>
       </c>
       <c r="F73">
-        <v>0.746406614780426</v>
+        <v>0.2213827520608902</v>
       </c>
       <c r="G73">
-        <v>0.6151475310325623</v>
+        <v>0.5500881671905518</v>
       </c>
       <c r="H73" t="s">
         <v>10</v>
       </c>
       <c r="I73">
-        <v>4.059774398803711</v>
+        <v>3.674150228500366</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B74">
-        <v>0.8696997761726379</v>
+        <v>0.5590777993202209</v>
       </c>
       <c r="C74">
-        <v>1.070242762565613</v>
+        <v>1.424061179161072</v>
       </c>
       <c r="D74">
-        <v>4.045622825622559</v>
+        <v>3.626932859420776</v>
       </c>
       <c r="E74">
-        <v>0.4656721949577332</v>
+        <v>0.3994297981262207</v>
       </c>
       <c r="F74">
-        <v>0.373986691236496</v>
+        <v>0.4005314111709595</v>
       </c>
       <c r="G74">
-        <v>0.4815391302108765</v>
+        <v>0.4494007229804993</v>
       </c>
       <c r="H74" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I74">
-        <v>4.045622825622559</v>
+        <v>3.626932859420776</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B75">
-        <v>1.541256189346313</v>
+        <v>1.000615477561951</v>
       </c>
       <c r="C75">
-        <v>0.1960794627666473</v>
+        <v>0.4275351464748383</v>
       </c>
       <c r="D75">
-        <v>3.969983100891113</v>
+        <v>3.609516143798828</v>
       </c>
       <c r="E75">
-        <v>0.7784076333045959</v>
+        <v>0.4393072128295898</v>
       </c>
       <c r="F75">
-        <v>0.2576448917388916</v>
+        <v>0.2486212402582169</v>
       </c>
       <c r="G75">
-        <v>0.4945489168167114</v>
+        <v>0.438384622335434</v>
       </c>
       <c r="H75" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I75">
-        <v>3.969983100891113</v>
+        <v>3.609516143798828</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B76">
-        <v>0.7354921698570251</v>
+        <v>0.3336067497730255</v>
       </c>
       <c r="C76">
-        <v>0.585275411605835</v>
+        <v>0.4892699420452118</v>
       </c>
       <c r="D76">
-        <v>3.968168497085571</v>
+        <v>3.602411270141602</v>
       </c>
       <c r="E76">
-        <v>0.5023262500762939</v>
+        <v>0.2409688085317612</v>
       </c>
       <c r="F76">
-        <v>0.402109295129776</v>
+        <v>0.5706766247749329</v>
       </c>
       <c r="G76">
-        <v>0.4295401871204376</v>
+        <v>0.5308374762535095</v>
       </c>
       <c r="H76" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I76">
-        <v>3.968168497085571</v>
+        <v>3.602411270141602</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B77">
-        <v>3.949311494827271</v>
+        <v>3.571057796478271</v>
       </c>
       <c r="C77">
-        <v>2.951563596725464</v>
+        <v>0.1704869121313095</v>
       </c>
       <c r="D77">
-        <v>0.5321440696716309</v>
+        <v>0.5966870784759521</v>
       </c>
       <c r="E77">
-        <v>0.7784076333045959</v>
+        <v>0.7817679643630981</v>
       </c>
       <c r="F77">
-        <v>0.5733299255371094</v>
+        <v>0.2187499701976776</v>
       </c>
       <c r="G77">
-        <v>0.3369401395320892</v>
+        <v>0.4292178452014923</v>
       </c>
       <c r="H77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I77">
-        <v>3.949311494827271</v>
+        <v>3.571057796478271</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B78">
-        <v>3.860986232757568</v>
+        <v>3.492010116577148</v>
       </c>
       <c r="C78">
-        <v>0.4052713513374329</v>
+        <v>0.2414712011814117</v>
       </c>
       <c r="D78">
-        <v>0.6216647028923035</v>
+        <v>0.9645367860794067</v>
       </c>
       <c r="E78">
-        <v>0.7784076333045959</v>
+        <v>0.7896054983139038</v>
       </c>
       <c r="F78">
-        <v>0.3095604479312897</v>
+        <v>0.2187499701976776</v>
       </c>
       <c r="G78">
-        <v>0.3194479942321777</v>
+        <v>0.3415709733963013</v>
       </c>
       <c r="H78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I78">
-        <v>3.860986232757568</v>
+        <v>3.492010116577148</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B79">
-        <v>0.5546631813049316</v>
+        <v>3.436897754669189</v>
       </c>
       <c r="C79">
-        <v>1.21626079082489</v>
+        <v>0.3438328206539154</v>
       </c>
       <c r="D79">
-        <v>3.801631927490234</v>
+        <v>0.9212982058525085</v>
       </c>
       <c r="E79">
-        <v>0.4169610440731049</v>
+        <v>0.4020107388496399</v>
       </c>
       <c r="F79">
-        <v>0.6471012830734253</v>
+        <v>0.3035051822662354</v>
       </c>
       <c r="G79">
-        <v>0.7396575212478638</v>
+        <v>0.439231812953949</v>
       </c>
       <c r="H79" t="s">
         <v>9</v>
       </c>
       <c r="I79">
-        <v>3.801631927490234</v>
+        <v>3.436897754669189</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B80">
-        <v>0.7740651965141296</v>
+        <v>0.5387656688690186</v>
       </c>
       <c r="C80">
-        <v>0.354597419500351</v>
+        <v>0.4251333475112915</v>
       </c>
       <c r="D80">
-        <v>3.797738075256348</v>
+        <v>3.434826850891113</v>
       </c>
       <c r="E80">
-        <v>0.5065588355064392</v>
+        <v>0.4787610471248627</v>
       </c>
       <c r="F80">
-        <v>0.4007653892040253</v>
+        <v>0.3960905969142914</v>
       </c>
       <c r="G80">
-        <v>0.648996114730835</v>
+        <v>0.7043770551681519</v>
       </c>
       <c r="H80" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I80">
-        <v>3.797738075256348</v>
+        <v>3.434826850891113</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -2738,57 +2738,57 @@
         <v>3</v>
       </c>
       <c r="B81">
-        <v>1.458858132362366</v>
+        <v>3.411182641983032</v>
       </c>
       <c r="C81">
-        <v>1.585588097572327</v>
+        <v>0.3434814214706421</v>
       </c>
       <c r="D81">
-        <v>3.740965843200684</v>
+        <v>0.4742518067359924</v>
       </c>
       <c r="E81">
-        <v>0.4470676779747009</v>
+        <v>0.70946204662323</v>
       </c>
       <c r="F81">
-        <v>0.4764663875102997</v>
+        <v>0.2314237654209137</v>
       </c>
       <c r="G81">
-        <v>0.4810720980167389</v>
+        <v>0.2187835574150085</v>
       </c>
       <c r="H81" t="s">
         <v>9</v>
       </c>
       <c r="I81">
-        <v>3.740965843200684</v>
+        <v>3.411182641983032</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B82">
-        <v>1.458858132362366</v>
+        <v>0.4360147416591644</v>
       </c>
       <c r="C82">
-        <v>3.720833539962769</v>
+        <v>0.5494910478591919</v>
       </c>
       <c r="D82">
-        <v>0.8919916152954102</v>
+        <v>3.348251342773438</v>
       </c>
       <c r="E82">
-        <v>0.4470676779747009</v>
+        <v>0.3783649802207947</v>
       </c>
       <c r="F82">
-        <v>0.3882851600646973</v>
+        <v>0.3679676353931427</v>
       </c>
       <c r="G82">
-        <v>0.3350296020507812</v>
+        <v>0.5356680750846863</v>
       </c>
       <c r="H82" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I82">
-        <v>3.720833539962769</v>
+        <v>3.348251342773438</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -2796,260 +2796,260 @@
         <v>3</v>
       </c>
       <c r="B83">
-        <v>3.682377815246582</v>
+        <v>0.8494998812675476</v>
       </c>
       <c r="C83">
-        <v>0.5623009204864502</v>
+        <v>3.248117446899414</v>
       </c>
       <c r="D83">
-        <v>0.4831186532974243</v>
+        <v>2.225080728530884</v>
       </c>
       <c r="E83">
-        <v>0.7784076333045959</v>
+        <v>0.6909928321838379</v>
       </c>
       <c r="F83">
-        <v>0.4530773162841797</v>
+        <v>0.4752231240272522</v>
       </c>
       <c r="G83">
-        <v>0.2690120339393616</v>
+        <v>0.703268826007843</v>
       </c>
       <c r="H83" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I83">
-        <v>3.682377815246582</v>
+        <v>3.248117446899414</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="B84">
-        <v>2.000677824020386</v>
+        <v>0.8190135359764099</v>
       </c>
       <c r="C84">
-        <v>0.6525818705558777</v>
+        <v>0.3441135287284851</v>
       </c>
       <c r="D84">
-        <v>3.654527187347412</v>
+        <v>3.215967416763306</v>
       </c>
       <c r="E84">
-        <v>0.6607242822647095</v>
+        <v>0.5348133444786072</v>
       </c>
       <c r="F84">
-        <v>0.6191713809967041</v>
+        <v>0.3804852366447449</v>
       </c>
       <c r="G84">
-        <v>0.5291274189949036</v>
+        <v>0.55064457654953</v>
       </c>
       <c r="H84" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I84">
-        <v>3.654527187347412</v>
+        <v>3.215967416763306</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B85">
-        <v>0.9421846270561218</v>
+        <v>0.8202193975448608</v>
       </c>
       <c r="C85">
-        <v>0.2499421238899231</v>
+        <v>0.4633361101150513</v>
       </c>
       <c r="D85">
-        <v>3.629386186599731</v>
+        <v>3.121118783950806</v>
       </c>
       <c r="E85">
-        <v>0.4864585399627686</v>
+        <v>0.4253511130809784</v>
       </c>
       <c r="F85">
-        <v>0.2829548418521881</v>
+        <v>0.371159553527832</v>
       </c>
       <c r="G85">
-        <v>0.5940791368484497</v>
+        <v>0.3667866289615631</v>
       </c>
       <c r="H85" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I85">
-        <v>3.629386186599731</v>
+        <v>3.121118783950806</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B86">
-        <v>0.4683996140956879</v>
+        <v>0.6299841403961182</v>
       </c>
       <c r="C86">
-        <v>0.2522758543491364</v>
+        <v>0.436733603477478</v>
       </c>
       <c r="D86">
-        <v>3.563722133636475</v>
+        <v>3.043490409851074</v>
       </c>
       <c r="E86">
-        <v>0.2689465582370758</v>
+        <v>0.4819014966487885</v>
       </c>
       <c r="F86">
-        <v>0.270305335521698</v>
+        <v>0.3729179501533508</v>
       </c>
       <c r="G86">
-        <v>0.6352455615997314</v>
+        <v>0.3363138735294342</v>
       </c>
       <c r="H86" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I86">
-        <v>3.563722133636475</v>
+        <v>3.043490409851074</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B87">
-        <v>1.732621908187866</v>
+        <v>0.6118919253349304</v>
       </c>
       <c r="C87">
-        <v>0.3043313026428223</v>
+        <v>1.046817541122437</v>
       </c>
       <c r="D87">
-        <v>3.546738624572754</v>
+        <v>3.034385442733765</v>
       </c>
       <c r="E87">
-        <v>0.7784076333045959</v>
+        <v>0.2363758981227875</v>
       </c>
       <c r="F87">
-        <v>0.2861186861991882</v>
+        <v>0.3723730146884918</v>
       </c>
       <c r="G87">
-        <v>0.4318214356899261</v>
+        <v>0.4756392538547516</v>
       </c>
       <c r="H87" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I87">
-        <v>3.546738624572754</v>
+        <v>3.034385442733765</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B88">
-        <v>1.458858132362366</v>
+        <v>0.4639895558357239</v>
       </c>
       <c r="C88">
-        <v>0.4773798286914825</v>
+        <v>0.8950289487838745</v>
       </c>
       <c r="D88">
-        <v>3.54163384437561</v>
+        <v>3.007312297821045</v>
       </c>
       <c r="E88">
-        <v>0.4470676779747009</v>
+        <v>0.4092554152011871</v>
       </c>
       <c r="F88">
-        <v>0.400321751832962</v>
+        <v>0.6800346970558167</v>
       </c>
       <c r="G88">
-        <v>0.4069793820381165</v>
+        <v>0.4359100759029388</v>
       </c>
       <c r="H88" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I88">
-        <v>3.54163384437561</v>
+        <v>3.007312297821045</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B89">
-        <v>0.7327709794044495</v>
+        <v>2.992449045181274</v>
       </c>
       <c r="C89">
-        <v>0.2616743445396423</v>
+        <v>0.2939099669456482</v>
       </c>
       <c r="D89">
-        <v>3.532993793487549</v>
+        <v>0.4744851589202881</v>
       </c>
       <c r="E89">
-        <v>0.4543758928775787</v>
+        <v>0.6522709727287292</v>
       </c>
       <c r="F89">
-        <v>0.2826698422431946</v>
+        <v>0.2448031902313232</v>
       </c>
       <c r="G89">
-        <v>0.4433211982250214</v>
+        <v>0.3413137197494507</v>
       </c>
       <c r="H89" t="s">
         <v>9</v>
       </c>
       <c r="I89">
-        <v>3.532993793487549</v>
+        <v>2.992449045181274</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B90">
-        <v>0.7645553946495056</v>
+        <v>2.992449045181274</v>
       </c>
       <c r="C90">
-        <v>0.5105603933334351</v>
+        <v>0.317261129617691</v>
       </c>
       <c r="D90">
-        <v>3.462240219116211</v>
+        <v>1.405728101730347</v>
       </c>
       <c r="E90">
-        <v>0.4702398180961609</v>
+        <v>0.6522709727287292</v>
       </c>
       <c r="F90">
-        <v>0.5122182369232178</v>
+        <v>0.3873101472854614</v>
       </c>
       <c r="G90">
-        <v>0.5849958062171936</v>
+        <v>0.7204980254173279</v>
       </c>
       <c r="H90" t="s">
         <v>9</v>
       </c>
       <c r="I90">
-        <v>3.462240219116211</v>
+        <v>2.992449045181274</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B91">
-        <v>0.6979904174804688</v>
+        <v>0.5214720964431763</v>
       </c>
       <c r="C91">
-        <v>0.2676239311695099</v>
+        <v>2.979122161865234</v>
       </c>
       <c r="D91">
-        <v>3.445563793182373</v>
+        <v>1.619511961936951</v>
       </c>
       <c r="E91">
-        <v>0.3645676076412201</v>
+        <v>0.3714911043643951</v>
       </c>
       <c r="F91">
-        <v>0.2474293112754822</v>
+        <v>0.3593218624591827</v>
       </c>
       <c r="G91">
-        <v>0.3839925825595856</v>
+        <v>0.438157320022583</v>
       </c>
       <c r="H91" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I91">
-        <v>3.445563793182373</v>
+        <v>2.979122161865234</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3057,260 +3057,260 @@
         <v>4</v>
       </c>
       <c r="B92">
-        <v>0.7714713215827942</v>
+        <v>2.943866968154907</v>
       </c>
       <c r="C92">
-        <v>0.3801865875720978</v>
+        <v>2.381513118743896</v>
       </c>
       <c r="D92">
-        <v>3.434888362884521</v>
+        <v>0.9079650640487671</v>
       </c>
       <c r="E92">
-        <v>0.4335650205612183</v>
+        <v>0.6522709727287292</v>
       </c>
       <c r="F92">
-        <v>0.3891852200031281</v>
+        <v>0.7612464427947998</v>
       </c>
       <c r="G92">
-        <v>0.506574809551239</v>
+        <v>0.6531309485435486</v>
       </c>
       <c r="H92" t="s">
         <v>9</v>
       </c>
       <c r="I92">
-        <v>3.434888362884521</v>
+        <v>2.943866968154907</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B93">
-        <v>0.6942785382270813</v>
+        <v>0.9457775950431824</v>
       </c>
       <c r="C93">
-        <v>3.424356937408447</v>
+        <v>2.883020639419556</v>
       </c>
       <c r="D93">
-        <v>1.091877460479736</v>
+        <v>1.116384983062744</v>
       </c>
       <c r="E93">
-        <v>0.4462517499923706</v>
+        <v>0.4528072774410248</v>
       </c>
       <c r="F93">
-        <v>0.7285653948783875</v>
+        <v>0.4209674298763275</v>
       </c>
       <c r="G93">
-        <v>0.4632879197597504</v>
+        <v>0.5802174806594849</v>
       </c>
       <c r="H93" t="s">
         <v>11</v>
       </c>
       <c r="I93">
-        <v>3.424356937408447</v>
+        <v>2.883020639419556</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B94">
-        <v>1.5652756690979</v>
+        <v>0.5562331080436707</v>
       </c>
       <c r="C94">
-        <v>0.2315281331539154</v>
+        <v>0.6611424684524536</v>
       </c>
       <c r="D94">
-        <v>3.412886381149292</v>
+        <v>2.880934953689575</v>
       </c>
       <c r="E94">
-        <v>0.4809494018554688</v>
+        <v>0.4064222872257233</v>
       </c>
       <c r="F94">
-        <v>0.2858741283416748</v>
+        <v>0.294289231300354</v>
       </c>
       <c r="G94">
-        <v>0.5669849514961243</v>
+        <v>0.4153705239295959</v>
       </c>
       <c r="H94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I94">
-        <v>3.412886381149292</v>
+        <v>2.880934953689575</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B95">
-        <v>1.458858132362366</v>
+        <v>1.014406442642212</v>
       </c>
       <c r="C95">
-        <v>0.1959111988544464</v>
+        <v>2.87935209274292</v>
       </c>
       <c r="D95">
-        <v>3.406586170196533</v>
+        <v>0.5729262828826904</v>
       </c>
       <c r="E95">
-        <v>0.4470676779747009</v>
+        <v>0.7149004936218262</v>
       </c>
       <c r="F95">
-        <v>0.243488684296608</v>
+        <v>0.7476269602775574</v>
       </c>
       <c r="G95">
-        <v>0.4878399968147278</v>
+        <v>0.2828547358512878</v>
       </c>
       <c r="H95" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I95">
-        <v>3.406586170196533</v>
+        <v>2.87935209274292</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B96">
-        <v>0.7836705446243286</v>
+        <v>1.804637670516968</v>
       </c>
       <c r="C96">
-        <v>0.3103288114070892</v>
+        <v>0.8272866606712341</v>
       </c>
       <c r="D96">
-        <v>3.376473903656006</v>
+        <v>2.852256536483765</v>
       </c>
       <c r="E96">
-        <v>0.4731191992759705</v>
+        <v>0.6381067633628845</v>
       </c>
       <c r="F96">
-        <v>0.3293386995792389</v>
+        <v>0.3091905117034912</v>
       </c>
       <c r="G96">
-        <v>0.5810909867286682</v>
+        <v>0.5176571011543274</v>
       </c>
       <c r="H96" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I96">
-        <v>3.376473903656006</v>
+        <v>2.852256536483765</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B97">
-        <v>0.541869580745697</v>
+        <v>2.842087745666504</v>
       </c>
       <c r="C97">
-        <v>3.372266292572021</v>
+        <v>0.2687933743000031</v>
       </c>
       <c r="D97">
-        <v>0.6124865412712097</v>
+        <v>1.252828359603882</v>
       </c>
       <c r="E97">
-        <v>0.3496139943599701</v>
+        <v>0.3324363529682159</v>
       </c>
       <c r="F97">
-        <v>0.364255964756012</v>
+        <v>0.2483253479003906</v>
       </c>
       <c r="G97">
-        <v>0.2815154790878296</v>
+        <v>0.5564073324203491</v>
       </c>
       <c r="H97" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I97">
-        <v>3.372266292572021</v>
+        <v>2.842087745666504</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B98">
-        <v>0.6642290949821472</v>
+        <v>2.840349435806274</v>
       </c>
       <c r="C98">
-        <v>3.362584352493286</v>
+        <v>0.707105815410614</v>
       </c>
       <c r="D98">
-        <v>0.798795223236084</v>
+        <v>0.6224014163017273</v>
       </c>
       <c r="E98">
-        <v>0.4297548234462738</v>
+        <v>0.7900606989860535</v>
       </c>
       <c r="F98">
-        <v>0.3620627522468567</v>
+        <v>0.6401103138923645</v>
       </c>
       <c r="G98">
-        <v>0.5793930888175964</v>
+        <v>0.4477150738239288</v>
       </c>
       <c r="H98" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I98">
-        <v>3.362584352493286</v>
+        <v>2.840349435806274</v>
       </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B99">
-        <v>3.342432737350464</v>
+        <v>2.840085983276367</v>
       </c>
       <c r="C99">
-        <v>0.3436686098575592</v>
+        <v>0.3279384970664978</v>
       </c>
       <c r="D99">
-        <v>1.305865049362183</v>
+        <v>0.7872990965843201</v>
       </c>
       <c r="E99">
-        <v>0.7722392678260803</v>
+        <v>0.7778476476669312</v>
       </c>
       <c r="F99">
-        <v>0.2990080416202545</v>
+        <v>0.3095730841159821</v>
       </c>
       <c r="G99">
-        <v>0.5823376178741455</v>
+        <v>0.4081725180149078</v>
       </c>
       <c r="H99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I99">
-        <v>3.342432737350464</v>
+        <v>2.840085983276367</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="A100">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B100">
-        <v>3.33725905418396</v>
+        <v>2.592391014099121</v>
       </c>
       <c r="C100">
-        <v>0.7231807708740234</v>
+        <v>0.2667898833751678</v>
       </c>
       <c r="D100">
-        <v>0.5747642517089844</v>
+        <v>2.789860010147095</v>
       </c>
       <c r="E100">
-        <v>0.7784076333045959</v>
+        <v>0.4781155586242676</v>
       </c>
       <c r="F100">
-        <v>0.4131025671958923</v>
+        <v>0.3587712943553925</v>
       </c>
       <c r="G100">
-        <v>0.3239488303661346</v>
+        <v>0.4303486049175262</v>
       </c>
       <c r="H100" t="s">
         <v>10</v>
       </c>
       <c r="I100">
-        <v>3.33725905418396</v>
+        <v>2.789860010147095</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -3318,28 +3318,28 @@
         <v>4</v>
       </c>
       <c r="B101">
-        <v>3.330070734024048</v>
+        <v>1.114575505256653</v>
       </c>
       <c r="C101">
-        <v>0.6396886706352234</v>
+        <v>2.780062437057495</v>
       </c>
       <c r="D101">
-        <v>0.7270520329475403</v>
+        <v>0.9403793215751648</v>
       </c>
       <c r="E101">
-        <v>0.7722392678260803</v>
+        <v>0.6707724928855896</v>
       </c>
       <c r="F101">
-        <v>0.7498457431793213</v>
+        <v>0.678011417388916</v>
       </c>
       <c r="G101">
-        <v>0.4278362691402435</v>
+        <v>0.5025174021720886</v>
       </c>
       <c r="H101" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I101">
-        <v>3.330070734024048</v>
+        <v>2.780062437057495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove highly co-related features
</commit_message>
<xml_diff>
--- a/results/recommendations.xlsx
+++ b/results/recommendations.xlsx
@@ -46,10 +46,10 @@
     <t>CC</t>
   </si>
   <si>
-    <t>CL</t>
+    <t>MF</t>
   </si>
   <si>
-    <t>MF</t>
+    <t>CL</t>
   </si>
 </sst>
 </file>
@@ -444,234 +444,234 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>72.32727813720703</v>
+        <v>58.73453521728516</v>
       </c>
       <c r="C2">
-        <v>0.3931759297847748</v>
+        <v>0.3948671221733093</v>
       </c>
       <c r="D2">
-        <v>1.174347400665283</v>
+        <v>1.898824095726013</v>
       </c>
       <c r="E2">
-        <v>0.4449374973773956</v>
+        <v>0.6844598054885864</v>
       </c>
       <c r="F2">
-        <v>0.3367405235767365</v>
+        <v>0.5057008862495422</v>
       </c>
       <c r="G2">
-        <v>0.2501336932182312</v>
+        <v>0.5635192394256592</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
       </c>
       <c r="I2">
-        <v>72.32727813720703</v>
+        <v>58.73453521728516</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>53.65043640136719</v>
+        <v>48.64484024047852</v>
       </c>
       <c r="C3">
-        <v>0.3969834446907043</v>
+        <v>0.2712957561016083</v>
       </c>
       <c r="D3">
-        <v>1.423470258712769</v>
+        <v>0.9193922877311707</v>
       </c>
       <c r="E3">
-        <v>0.625212550163269</v>
+        <v>0.2992496490478516</v>
       </c>
       <c r="F3">
-        <v>0.5093652606010437</v>
+        <v>0.2411055266857147</v>
       </c>
       <c r="G3">
-        <v>0.6683977842330933</v>
+        <v>0.4322488307952881</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>
       </c>
       <c r="I3">
-        <v>53.65043640136719</v>
+        <v>48.64484024047852</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>32.23302841186523</v>
+        <v>1.406337022781372</v>
       </c>
       <c r="C4">
-        <v>0.2178645431995392</v>
+        <v>36.14056777954102</v>
       </c>
       <c r="D4">
-        <v>1.396708488464355</v>
+        <v>1.142784595489502</v>
       </c>
       <c r="E4">
-        <v>0.6679288148880005</v>
+        <v>0.4898841083049774</v>
       </c>
       <c r="F4">
-        <v>0.2088626623153687</v>
+        <v>0.410150021314621</v>
       </c>
       <c r="G4">
-        <v>0.4115189611911774</v>
+        <v>0.4322344958782196</v>
       </c>
       <c r="H4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I4">
-        <v>32.23302841186523</v>
+        <v>36.14056777954102</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>24.36797904968262</v>
+        <v>0.6314648985862732</v>
       </c>
       <c r="C5">
-        <v>0.800474226474762</v>
+        <v>27.6715087890625</v>
       </c>
       <c r="D5">
-        <v>1.760137557983398</v>
+        <v>0.6629825830459595</v>
       </c>
       <c r="E5">
-        <v>0.504950225353241</v>
+        <v>0.4526007473468781</v>
       </c>
       <c r="F5">
-        <v>0.6800346970558167</v>
+        <v>0.3140368461608887</v>
       </c>
       <c r="G5">
-        <v>0.3917422890663147</v>
+        <v>0.3267242908477783</v>
       </c>
       <c r="H5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I5">
-        <v>24.36797904968262</v>
+        <v>27.6715087890625</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>23.42295074462891</v>
+        <v>2.223084688186646</v>
       </c>
       <c r="C6">
-        <v>0.6047609448432922</v>
+        <v>23.13810157775879</v>
       </c>
       <c r="D6">
-        <v>0.4544323682785034</v>
+        <v>0.6864070892333984</v>
       </c>
       <c r="E6">
-        <v>0.485367476940155</v>
+        <v>0.7796120643615723</v>
       </c>
       <c r="F6">
-        <v>0.551078200340271</v>
+        <v>0.6819660663604736</v>
       </c>
       <c r="G6">
-        <v>0.2117873728275299</v>
+        <v>0.4937565624713898</v>
       </c>
       <c r="H6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I6">
-        <v>23.42295074462891</v>
+        <v>23.13810157775879</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B7">
-        <v>0.4489038586616516</v>
+        <v>22.84070205688477</v>
       </c>
       <c r="C7">
-        <v>0.291985422372818</v>
+        <v>7.970110893249512</v>
       </c>
       <c r="D7">
-        <v>13.98909187316895</v>
+        <v>0.5689920783042908</v>
       </c>
       <c r="E7">
-        <v>0.3867040872573853</v>
+        <v>0.5439000725746155</v>
       </c>
       <c r="F7">
-        <v>0.2270368933677673</v>
+        <v>0.3524862825870514</v>
       </c>
       <c r="G7">
-        <v>0.7905167937278748</v>
+        <v>0.2781054079532623</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I7">
-        <v>13.98909187316895</v>
+        <v>22.84070205688477</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>1.063194513320923</v>
+        <v>14.52297019958496</v>
       </c>
       <c r="C8">
-        <v>0.5582491755485535</v>
+        <v>0.3334438800811768</v>
       </c>
       <c r="D8">
-        <v>13.95850276947021</v>
+        <v>1.187095403671265</v>
       </c>
       <c r="E8">
-        <v>0.7681990265846252</v>
+        <v>0.4677047729492188</v>
       </c>
       <c r="F8">
-        <v>0.4398095607757568</v>
+        <v>0.403346449136734</v>
       </c>
       <c r="G8">
-        <v>0.2557952702045441</v>
+        <v>0.584485650062561</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I8">
-        <v>13.95850276947021</v>
+        <v>14.52297019958496</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>0.492353767156601</v>
+        <v>0.4679007530212402</v>
       </c>
       <c r="C9">
-        <v>0.3013112246990204</v>
+        <v>0.323331743478775</v>
       </c>
       <c r="D9">
-        <v>13.58257961273193</v>
+        <v>13.62450504302979</v>
       </c>
       <c r="E9">
-        <v>0.3738916516304016</v>
+        <v>0.3706963956356049</v>
       </c>
       <c r="F9">
-        <v>0.3235803246498108</v>
+        <v>0.3065899014472961</v>
       </c>
       <c r="G9">
-        <v>0.7615388631820679</v>
+        <v>0.7852787971496582</v>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I9">
-        <v>13.58257961273193</v>
+        <v>13.62450504302979</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -679,115 +679,115 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <v>12.8204517364502</v>
+        <v>1.115027785301208</v>
       </c>
       <c r="C10">
-        <v>0.3878532350063324</v>
+        <v>0.3553973138332367</v>
       </c>
       <c r="D10">
-        <v>0.6051624417304993</v>
+        <v>13.50553417205811</v>
       </c>
       <c r="E10">
-        <v>0.7900606989860535</v>
+        <v>0.7994129657745361</v>
       </c>
       <c r="F10">
-        <v>0.2662014365196228</v>
+        <v>0.2742395102977753</v>
       </c>
       <c r="G10">
-        <v>0.2279759347438812</v>
+        <v>0.2474944293498993</v>
       </c>
       <c r="H10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I10">
-        <v>12.8204517364502</v>
+        <v>13.50553417205811</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>12.31007862091064</v>
+        <v>12.42453098297119</v>
       </c>
       <c r="C11">
-        <v>0.3864842355251312</v>
+        <v>0.3808318972587585</v>
       </c>
       <c r="D11">
-        <v>0.3260757923126221</v>
+        <v>0.6078271865844727</v>
       </c>
       <c r="E11">
-        <v>0.7586089372634888</v>
+        <v>0.7896831035614014</v>
       </c>
       <c r="F11">
-        <v>0.3500140607357025</v>
+        <v>0.2955687940120697</v>
       </c>
       <c r="G11">
-        <v>0.2345577031373978</v>
+        <v>0.2687463760375977</v>
       </c>
       <c r="H11" t="s">
         <v>9</v>
       </c>
       <c r="I11">
-        <v>12.31007862091064</v>
+        <v>12.42453098297119</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12">
-        <v>9.46833610534668</v>
+        <v>0.8802586793899536</v>
       </c>
       <c r="C12">
-        <v>0.2600335776805878</v>
+        <v>0.3180978894233704</v>
       </c>
       <c r="D12">
-        <v>0.6422207355499268</v>
+        <v>11.12108612060547</v>
       </c>
       <c r="E12">
-        <v>0.5103054642677307</v>
+        <v>0.6442665457725525</v>
       </c>
       <c r="F12">
-        <v>0.2433930039405823</v>
+        <v>0.3016270399093628</v>
       </c>
       <c r="G12">
-        <v>0.2926400303840637</v>
+        <v>0.6361361742019653</v>
       </c>
       <c r="H12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I12">
-        <v>9.46833610534668</v>
+        <v>11.12108612060547</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>0.5113710165023804</v>
+        <v>0.492921382188797</v>
       </c>
       <c r="C13">
-        <v>0.2278967499732971</v>
+        <v>0.4362378716468811</v>
       </c>
       <c r="D13">
-        <v>9.077680587768555</v>
+        <v>10.96627998352051</v>
       </c>
       <c r="E13">
-        <v>0.4055269956588745</v>
+        <v>0.3977853953838348</v>
       </c>
       <c r="F13">
-        <v>0.2447399944067001</v>
+        <v>0.3661500811576843</v>
       </c>
       <c r="G13">
-        <v>0.6707048416137695</v>
+        <v>0.6640705466270447</v>
       </c>
       <c r="H13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I13">
-        <v>9.077680587768555</v>
+        <v>10.96627998352051</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -795,144 +795,144 @@
         <v>6</v>
       </c>
       <c r="B14">
-        <v>8.579387664794922</v>
+        <v>0.5673749446868896</v>
       </c>
       <c r="C14">
-        <v>0.3155757784843445</v>
+        <v>0.3003255724906921</v>
       </c>
       <c r="D14">
-        <v>0.6188979148864746</v>
+        <v>8.970088005065918</v>
       </c>
       <c r="E14">
-        <v>0.5287050008773804</v>
+        <v>0.4066644310951233</v>
       </c>
       <c r="F14">
-        <v>0.2049365341663361</v>
+        <v>0.2847749590873718</v>
       </c>
       <c r="G14">
-        <v>0.2948892712593079</v>
+        <v>0.5580616593360901</v>
       </c>
       <c r="H14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I14">
-        <v>8.579387664794922</v>
+        <v>8.970088005065918</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>1.013941764831543</v>
+        <v>8.934244155883789</v>
       </c>
       <c r="C15">
-        <v>8.156551361083984</v>
+        <v>0.252127468585968</v>
       </c>
       <c r="D15">
-        <v>0.9895534515380859</v>
+        <v>0.6064607501029968</v>
       </c>
       <c r="E15">
-        <v>0.5048841834068298</v>
+        <v>0.49869105219841</v>
       </c>
       <c r="F15">
-        <v>0.5306404232978821</v>
+        <v>0.2295928448438644</v>
       </c>
       <c r="G15">
-        <v>0.4500592648983002</v>
+        <v>0.2724359631538391</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I15">
-        <v>8.156551361083984</v>
+        <v>8.934244155883789</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>0.4722757935523987</v>
+        <v>0.6007726788520813</v>
       </c>
       <c r="C16">
-        <v>0.6049237251281738</v>
+        <v>8.621372222900391</v>
       </c>
       <c r="D16">
-        <v>8.075596809387207</v>
+        <v>1.790491223335266</v>
       </c>
       <c r="E16">
-        <v>0.3082205653190613</v>
+        <v>0.4709456264972687</v>
       </c>
       <c r="F16">
-        <v>0.6395595073699951</v>
+        <v>0.5936911106109619</v>
       </c>
       <c r="G16">
-        <v>0.7907135486602783</v>
+        <v>0.5615100860595703</v>
       </c>
       <c r="H16" t="s">
         <v>10</v>
       </c>
       <c r="I16">
-        <v>8.075596809387207</v>
+        <v>8.621372222900391</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B17">
-        <v>7.924840927124023</v>
+        <v>0.9039761424064636</v>
       </c>
       <c r="C17">
-        <v>0.2855639159679413</v>
+        <v>7.847912788391113</v>
       </c>
       <c r="D17">
-        <v>0.7000500559806824</v>
+        <v>1.55403733253479</v>
       </c>
       <c r="E17">
-        <v>0.4271172285079956</v>
+        <v>0.3449106514453888</v>
       </c>
       <c r="F17">
-        <v>0.2843851447105408</v>
+        <v>0.3470819294452667</v>
       </c>
       <c r="G17">
-        <v>0.3179340660572052</v>
+        <v>0.4594657719135284</v>
       </c>
       <c r="H17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I17">
-        <v>7.924840927124023</v>
+        <v>7.847912788391113</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <v>0.4288828670978546</v>
+        <v>0.9129478931427002</v>
       </c>
       <c r="C18">
-        <v>7.879054546356201</v>
+        <v>0.3151211738586426</v>
       </c>
       <c r="D18">
-        <v>0.6754574775695801</v>
+        <v>7.667858600616455</v>
       </c>
       <c r="E18">
-        <v>0.2135587930679321</v>
+        <v>0.5356919169425964</v>
       </c>
       <c r="F18">
-        <v>0.3484592139720917</v>
+        <v>0.269353061914444</v>
       </c>
       <c r="G18">
-        <v>0.4210911691188812</v>
+        <v>0.694905698299408</v>
       </c>
       <c r="H18" t="s">
         <v>11</v>
       </c>
       <c r="I18">
-        <v>7.879054546356201</v>
+        <v>7.667858600616455</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -940,115 +940,115 @@
         <v>3</v>
       </c>
       <c r="B19">
-        <v>0.4235605001449585</v>
+        <v>7.655832767486572</v>
       </c>
       <c r="C19">
-        <v>0.2657084167003632</v>
+        <v>0.5731478333473206</v>
       </c>
       <c r="D19">
-        <v>7.855395793914795</v>
+        <v>1.419181346893311</v>
       </c>
       <c r="E19">
-        <v>0.3216502964496613</v>
+        <v>0.4888263940811157</v>
       </c>
       <c r="F19">
-        <v>0.2725946307182312</v>
+        <v>0.4164429903030396</v>
       </c>
       <c r="G19">
-        <v>0.4887738823890686</v>
+        <v>0.5259780883789062</v>
       </c>
       <c r="H19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I19">
-        <v>7.855395793914795</v>
+        <v>7.655832767486572</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B20">
-        <v>0.8569344878196716</v>
+        <v>0.7987030148506165</v>
       </c>
       <c r="C20">
-        <v>0.2625806331634521</v>
+        <v>0.852562427520752</v>
       </c>
       <c r="D20">
-        <v>7.817061901092529</v>
+        <v>7.605278968811035</v>
       </c>
       <c r="E20">
-        <v>0.5143541097640991</v>
+        <v>0.5845754742622375</v>
       </c>
       <c r="F20">
-        <v>0.3986643850803375</v>
+        <v>0.6679509878158569</v>
       </c>
       <c r="G20">
-        <v>0.6889245510101318</v>
+        <v>0.6722796559333801</v>
       </c>
       <c r="H20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I20">
-        <v>7.817061901092529</v>
+        <v>7.605278968811035</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B21">
-        <v>0.6891282796859741</v>
+        <v>7.456857681274414</v>
       </c>
       <c r="C21">
-        <v>0.2120774835348129</v>
+        <v>0.3701926171779633</v>
       </c>
       <c r="D21">
-        <v>7.23508882522583</v>
+        <v>0.3420864343643188</v>
       </c>
       <c r="E21">
-        <v>0.4136325120925903</v>
+        <v>0.473945826292038</v>
       </c>
       <c r="F21">
-        <v>0.2275406420230865</v>
+        <v>0.2695298492908478</v>
       </c>
       <c r="G21">
-        <v>0.7843341827392578</v>
+        <v>0.2460747063159943</v>
       </c>
       <c r="H21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I21">
-        <v>7.23508882522583</v>
+        <v>7.456857681274414</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B22">
-        <v>0.8474979400634766</v>
+        <v>0.7999568581581116</v>
       </c>
       <c r="C22">
-        <v>0.4901507198810577</v>
+        <v>0.5827192068099976</v>
       </c>
       <c r="D22">
-        <v>7.13730525970459</v>
+        <v>7.189822673797607</v>
       </c>
       <c r="E22">
-        <v>0.4080877304077148</v>
+        <v>0.62442547082901</v>
       </c>
       <c r="F22">
-        <v>0.4433773756027222</v>
+        <v>0.4454778432846069</v>
       </c>
       <c r="G22">
-        <v>0.7709833383560181</v>
+        <v>0.7852787971496582</v>
       </c>
       <c r="H22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I22">
-        <v>7.13730525970459</v>
+        <v>7.189822673797607</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1056,144 +1056,144 @@
         <v>4</v>
       </c>
       <c r="B23">
-        <v>0.4259302020072937</v>
+        <v>0.3088406920433044</v>
       </c>
       <c r="C23">
-        <v>0.3195417821407318</v>
+        <v>0.3222076296806335</v>
       </c>
       <c r="D23">
-        <v>6.989850521087646</v>
+        <v>7.120708465576172</v>
       </c>
       <c r="E23">
-        <v>0.328326940536499</v>
+        <v>0.2362249344587326</v>
       </c>
       <c r="F23">
-        <v>0.3069196343421936</v>
+        <v>0.2332487404346466</v>
       </c>
       <c r="G23">
-        <v>0.7950443029403687</v>
+        <v>0.7868634462356567</v>
       </c>
       <c r="H23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I23">
-        <v>6.989850521087646</v>
+        <v>7.120708465576172</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B24">
-        <v>0.3423245549201965</v>
+        <v>0.6930333971977234</v>
       </c>
       <c r="C24">
-        <v>0.9769492149353027</v>
+        <v>2.002154588699341</v>
       </c>
       <c r="D24">
-        <v>6.500402927398682</v>
+        <v>6.969654083251953</v>
       </c>
       <c r="E24">
-        <v>0.2742345333099365</v>
+        <v>0.2133300602436066</v>
       </c>
       <c r="F24">
-        <v>0.4473406076431274</v>
+        <v>0.5228955745697021</v>
       </c>
       <c r="G24">
-        <v>0.7764785885810852</v>
+        <v>0.6843295097351074</v>
       </c>
       <c r="H24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I24">
-        <v>6.500402927398682</v>
+        <v>6.969654083251953</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B25">
-        <v>0.9134219288825989</v>
+        <v>6.184057712554932</v>
       </c>
       <c r="C25">
-        <v>6.426394939422607</v>
+        <v>0.4078543186187744</v>
       </c>
       <c r="D25">
-        <v>0.8856394290924072</v>
+        <v>1.749161958694458</v>
       </c>
       <c r="E25">
-        <v>0.6208049654960632</v>
+        <v>0.7994129657745361</v>
       </c>
       <c r="F25">
-        <v>0.5612607598304749</v>
+        <v>0.3328530490398407</v>
       </c>
       <c r="G25">
-        <v>0.437241792678833</v>
+        <v>0.6131638884544373</v>
       </c>
       <c r="H25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I25">
-        <v>6.426394939422607</v>
+        <v>6.184057712554932</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>0.4286714494228363</v>
+        <v>6.178353309631348</v>
       </c>
       <c r="C26">
-        <v>0.6489058136940002</v>
+        <v>0.3134379088878632</v>
       </c>
       <c r="D26">
-        <v>6.41123628616333</v>
+        <v>0.605269193649292</v>
       </c>
       <c r="E26">
-        <v>0.3099444806575775</v>
+        <v>0.3455123603343964</v>
       </c>
       <c r="F26">
-        <v>0.3972028791904449</v>
+        <v>0.2814735770225525</v>
       </c>
       <c r="G26">
-        <v>0.7949239015579224</v>
+        <v>0.3298624753952026</v>
       </c>
       <c r="H26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I26">
-        <v>6.41123628616333</v>
+        <v>6.178353309631348</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B27">
-        <v>4.518557548522949</v>
+        <v>0.31699338555336</v>
       </c>
       <c r="C27">
-        <v>1.022661924362183</v>
+        <v>0.3054425716400146</v>
       </c>
       <c r="D27">
-        <v>6.39005184173584</v>
+        <v>6.100268363952637</v>
       </c>
       <c r="E27">
-        <v>0.2781537175178528</v>
+        <v>0.2410591095685959</v>
       </c>
       <c r="F27">
-        <v>0.4067932367324829</v>
+        <v>0.2596114277839661</v>
       </c>
       <c r="G27">
-        <v>0.771868109703064</v>
+        <v>0.7341726422309875</v>
       </c>
       <c r="H27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I27">
-        <v>6.39005184173584</v>
+        <v>6.100268363952637</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1201,202 +1201,202 @@
         <v>2</v>
       </c>
       <c r="B28">
-        <v>0.7308862805366516</v>
+        <v>0.7223234176635742</v>
       </c>
       <c r="C28">
-        <v>0.4886845350265503</v>
+        <v>6.063041687011719</v>
       </c>
       <c r="D28">
-        <v>6.272773742675781</v>
+        <v>1.466445088386536</v>
       </c>
       <c r="E28">
-        <v>0.3519368171691895</v>
+        <v>0.3944889903068542</v>
       </c>
       <c r="F28">
-        <v>0.4280272424221039</v>
+        <v>0.3765509724617004</v>
       </c>
       <c r="G28">
-        <v>0.7160928845405579</v>
+        <v>0.5653538107872009</v>
       </c>
       <c r="H28" t="s">
         <v>10</v>
       </c>
       <c r="I28">
-        <v>6.272773742675781</v>
+        <v>6.063041687011719</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B29">
-        <v>3.351975917816162</v>
+        <v>0.6834059357643127</v>
       </c>
       <c r="C29">
-        <v>0.9243535995483398</v>
+        <v>0.3115998804569244</v>
       </c>
       <c r="D29">
-        <v>6.234553337097168</v>
+        <v>5.979367256164551</v>
       </c>
       <c r="E29">
-        <v>0.3920775055885315</v>
+        <v>0.5369131565093994</v>
       </c>
       <c r="F29">
-        <v>0.4871386289596558</v>
+        <v>0.295465499162674</v>
       </c>
       <c r="G29">
-        <v>0.792801558971405</v>
+        <v>0.6910262107849121</v>
       </c>
       <c r="H29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I29">
-        <v>6.234553337097168</v>
+        <v>5.979367256164551</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30">
-        <v>0.6135110855102539</v>
+        <v>0.5970554351806641</v>
       </c>
       <c r="C30">
-        <v>0.7021892070770264</v>
+        <v>5.796629905700684</v>
       </c>
       <c r="D30">
-        <v>6.010499954223633</v>
+        <v>0.7099209427833557</v>
       </c>
       <c r="E30">
-        <v>0.4375878572463989</v>
+        <v>0.561957836151123</v>
       </c>
       <c r="F30">
-        <v>0.5093652606010437</v>
+        <v>0.2673864960670471</v>
       </c>
       <c r="G30">
-        <v>0.6640572547912598</v>
+        <v>0.3283736705780029</v>
       </c>
       <c r="H30" t="s">
         <v>10</v>
       </c>
       <c r="I30">
-        <v>6.010499954223633</v>
+        <v>5.796629905700684</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B31">
-        <v>0.5407677888870239</v>
+        <v>5.607229709625244</v>
       </c>
       <c r="C31">
-        <v>0.5786744356155396</v>
+        <v>0.1740079373121262</v>
       </c>
       <c r="D31">
-        <v>5.961269378662109</v>
+        <v>0.875428318977356</v>
       </c>
       <c r="E31">
-        <v>0.3729904890060425</v>
+        <v>0.4835149943828583</v>
       </c>
       <c r="F31">
-        <v>0.5064505338668823</v>
+        <v>0.2289658486843109</v>
       </c>
       <c r="G31">
-        <v>0.5512764453887939</v>
+        <v>0.3849727213382721</v>
       </c>
       <c r="H31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I31">
-        <v>5.961269378662109</v>
+        <v>5.607229709625244</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32">
-        <v>0.5723186731338501</v>
+        <v>2.391289472579956</v>
       </c>
       <c r="C32">
-        <v>0.2942241132259369</v>
+        <v>0.857571005821228</v>
       </c>
       <c r="D32">
-        <v>5.89526891708374</v>
+        <v>5.527441024780273</v>
       </c>
       <c r="E32">
-        <v>0.4138064682483673</v>
+        <v>0.3109385371208191</v>
       </c>
       <c r="F32">
-        <v>0.2379521727561951</v>
+        <v>0.5651676058769226</v>
       </c>
       <c r="G32">
-        <v>0.7934637069702148</v>
+        <v>0.7868712544441223</v>
       </c>
       <c r="H32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I32">
-        <v>5.89526891708374</v>
+        <v>5.527441024780273</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B33">
-        <v>1.42775297164917</v>
+        <v>0.7702404260635376</v>
       </c>
       <c r="C33">
-        <v>0.2904433310031891</v>
+        <v>0.346843957901001</v>
       </c>
       <c r="D33">
-        <v>5.678623199462891</v>
+        <v>5.498863697052002</v>
       </c>
       <c r="E33">
-        <v>0.5628227591514587</v>
+        <v>0.4465059041976929</v>
       </c>
       <c r="F33">
-        <v>0.2187499701976776</v>
+        <v>0.2964684367179871</v>
       </c>
       <c r="G33">
-        <v>0.616786003112793</v>
+        <v>0.7369493246078491</v>
       </c>
       <c r="H33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I33">
-        <v>5.678623199462891</v>
+        <v>5.498863697052002</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B34">
-        <v>0.4741286337375641</v>
+        <v>0.5182864665985107</v>
       </c>
       <c r="C34">
-        <v>0.2034213691949844</v>
+        <v>0.3669725954532623</v>
       </c>
       <c r="D34">
-        <v>5.659033298492432</v>
+        <v>5.48089599609375</v>
       </c>
       <c r="E34">
-        <v>0.3426439464092255</v>
+        <v>0.4128663539886475</v>
       </c>
       <c r="F34">
-        <v>0.2184557020664215</v>
+        <v>0.2876479625701904</v>
       </c>
       <c r="G34">
-        <v>0.3497738838195801</v>
+        <v>0.6944669485092163</v>
       </c>
       <c r="H34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I34">
-        <v>5.659033298492432</v>
+        <v>5.48089599609375</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1404,318 +1404,318 @@
         <v>2</v>
       </c>
       <c r="B35">
-        <v>0.4724365472793579</v>
+        <v>0.9514337778091431</v>
       </c>
       <c r="C35">
-        <v>0.5082722306251526</v>
+        <v>0.5556274056434631</v>
       </c>
       <c r="D35">
-        <v>5.528110504150391</v>
+        <v>5.312206745147705</v>
       </c>
       <c r="E35">
-        <v>0.2475945949554443</v>
+        <v>0.4395436644554138</v>
       </c>
       <c r="F35">
-        <v>0.309226006269455</v>
+        <v>0.4300339221954346</v>
       </c>
       <c r="G35">
-        <v>0.5096895694732666</v>
+        <v>0.6487395763397217</v>
       </c>
       <c r="H35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I35">
-        <v>5.528110504150391</v>
+        <v>5.312206745147705</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B36">
-        <v>0.5826843976974487</v>
+        <v>0.5862721800804138</v>
       </c>
       <c r="C36">
-        <v>0.276839941740036</v>
+        <v>0.4320283532142639</v>
       </c>
       <c r="D36">
-        <v>5.474831581115723</v>
+        <v>5.309828758239746</v>
       </c>
       <c r="E36">
-        <v>0.4436034560203552</v>
+        <v>0.4567930698394775</v>
       </c>
       <c r="F36">
-        <v>0.2909498810768127</v>
+        <v>0.3169446885585785</v>
       </c>
       <c r="G36">
-        <v>0.6266071200370789</v>
+        <v>0.7868712544441223</v>
       </c>
       <c r="H36" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I36">
-        <v>5.474831581115723</v>
+        <v>5.309828758239746</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B37">
-        <v>0.7513706684112549</v>
+        <v>2.508394479751587</v>
       </c>
       <c r="C37">
-        <v>0.4133648872375488</v>
+        <v>0.6086794137954712</v>
       </c>
       <c r="D37">
-        <v>5.345963478088379</v>
+        <v>5.293807506561279</v>
       </c>
       <c r="E37">
-        <v>0.4678671956062317</v>
+        <v>0.7994129657745361</v>
       </c>
       <c r="F37">
-        <v>0.3243132531642914</v>
+        <v>0.3274702131748199</v>
       </c>
       <c r="G37">
-        <v>0.7790641188621521</v>
+        <v>0.5537298917770386</v>
       </c>
       <c r="H37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I37">
-        <v>5.345963478088379</v>
+        <v>5.293807506561279</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B38">
-        <v>0.477464884519577</v>
+        <v>2.539978265762329</v>
       </c>
       <c r="C38">
-        <v>0.3393128514289856</v>
+        <v>0.8371579051017761</v>
       </c>
       <c r="D38">
-        <v>5.32615852355957</v>
+        <v>5.278081893920898</v>
       </c>
       <c r="E38">
-        <v>0.3625850975513458</v>
+        <v>0.3617963790893555</v>
       </c>
       <c r="F38">
-        <v>0.3104285597801208</v>
+        <v>0.5439035892486572</v>
       </c>
       <c r="G38">
-        <v>0.7024275064468384</v>
+        <v>0.7776456475257874</v>
       </c>
       <c r="H38" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I38">
-        <v>5.32615852355957</v>
+        <v>5.278081893920898</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B39">
-        <v>1.231008648872375</v>
+        <v>1.330970883369446</v>
       </c>
       <c r="C39">
-        <v>0.4923030138015747</v>
+        <v>0.3939110934734344</v>
       </c>
       <c r="D39">
-        <v>5.163406848907471</v>
+        <v>5.256078243255615</v>
       </c>
       <c r="E39">
-        <v>0.4231030941009521</v>
+        <v>0.4344120621681213</v>
       </c>
       <c r="F39">
-        <v>0.2708915174007416</v>
+        <v>0.3066438436508179</v>
       </c>
       <c r="G39">
-        <v>0.4638983011245728</v>
+        <v>0.634662926197052</v>
       </c>
       <c r="H39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I39">
-        <v>5.163406848907471</v>
+        <v>5.256078243255615</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B40">
-        <v>0.3245489597320557</v>
+        <v>0.5166853666305542</v>
       </c>
       <c r="C40">
-        <v>0.2872713804244995</v>
+        <v>5.228996753692627</v>
       </c>
       <c r="D40">
-        <v>5.117724895477295</v>
+        <v>0.9659311175346375</v>
       </c>
       <c r="E40">
-        <v>0.2352232336997986</v>
+        <v>0.3193460404872894</v>
       </c>
       <c r="F40">
-        <v>0.2174950242042542</v>
+        <v>0.4398955404758453</v>
       </c>
       <c r="G40">
-        <v>0.7615388631820679</v>
+        <v>0.4031373560428619</v>
       </c>
       <c r="H40" t="s">
         <v>10</v>
       </c>
       <c r="I40">
-        <v>5.117724895477295</v>
+        <v>5.228996753692627</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B41">
-        <v>5.069324493408203</v>
+        <v>0.9022312760353088</v>
       </c>
       <c r="C41">
-        <v>0.3780682682991028</v>
+        <v>2.041418552398682</v>
       </c>
       <c r="D41">
-        <v>2.497116088867188</v>
+        <v>5.138351917266846</v>
       </c>
       <c r="E41">
-        <v>0.3120578825473785</v>
+        <v>0.407346099615097</v>
       </c>
       <c r="F41">
-        <v>0.3004328608512878</v>
+        <v>0.3328530490398407</v>
       </c>
       <c r="G41">
-        <v>0.7701890468597412</v>
+        <v>0.4237348735332489</v>
       </c>
       <c r="H41" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I41">
-        <v>5.069324493408203</v>
+        <v>5.138351917266846</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B42">
-        <v>0.6439355611801147</v>
+        <v>5.063946723937988</v>
       </c>
       <c r="C42">
-        <v>0.6781551241874695</v>
+        <v>0.5558042526245117</v>
       </c>
       <c r="D42">
-        <v>5.00117301940918</v>
+        <v>0.967124879360199</v>
       </c>
       <c r="E42">
-        <v>0.4600559175014496</v>
+        <v>0.4590834975242615</v>
       </c>
       <c r="F42">
-        <v>0.3837210834026337</v>
+        <v>0.3888571560382843</v>
       </c>
       <c r="G42">
-        <v>0.7934637069702148</v>
+        <v>0.511224091053009</v>
       </c>
       <c r="H42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I42">
-        <v>5.00117301940918</v>
+        <v>5.063946723937988</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B43">
-        <v>0.2785486280918121</v>
+        <v>0.5900753140449524</v>
       </c>
       <c r="C43">
-        <v>0.2701749503612518</v>
+        <v>0.847577691078186</v>
       </c>
       <c r="D43">
-        <v>5.00107479095459</v>
+        <v>4.998666286468506</v>
       </c>
       <c r="E43">
-        <v>0.227186307311058</v>
+        <v>0.4591104984283447</v>
       </c>
       <c r="F43">
-        <v>0.2877107560634613</v>
+        <v>0.6280261278152466</v>
       </c>
       <c r="G43">
-        <v>0.7937372326850891</v>
+        <v>0.5891149640083313</v>
       </c>
       <c r="H43" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I43">
-        <v>5.00107479095459</v>
+        <v>4.998666286468506</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="B44">
-        <v>0.4069178104400635</v>
+        <v>0.9714727401733398</v>
       </c>
       <c r="C44">
-        <v>1.08289909362793</v>
+        <v>0.2496456652879715</v>
       </c>
       <c r="D44">
-        <v>4.974560260772705</v>
+        <v>4.991943359375</v>
       </c>
       <c r="E44">
-        <v>0.263069212436676</v>
+        <v>0.5397734642028809</v>
       </c>
       <c r="F44">
-        <v>0.5266286730766296</v>
+        <v>0.2831456065177917</v>
       </c>
       <c r="G44">
-        <v>0.6561864614486694</v>
+        <v>0.6954079270362854</v>
       </c>
       <c r="H44" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I44">
-        <v>4.974560260772705</v>
+        <v>4.991943359375</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B45">
-        <v>1.354509115219116</v>
+        <v>0.6918811798095703</v>
       </c>
       <c r="C45">
-        <v>0.3035514950752258</v>
+        <v>0.390522301197052</v>
       </c>
       <c r="D45">
-        <v>4.831519603729248</v>
+        <v>4.939728260040283</v>
       </c>
       <c r="E45">
-        <v>0.4655507504940033</v>
+        <v>0.3545735478401184</v>
       </c>
       <c r="F45">
-        <v>0.3010125458240509</v>
+        <v>0.324461042881012</v>
       </c>
       <c r="G45">
-        <v>0.6119588017463684</v>
+        <v>0.7916851043701172</v>
       </c>
       <c r="H45" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I45">
-        <v>4.831519603729248</v>
+        <v>4.939728260040283</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1723,202 +1723,202 @@
         <v>3</v>
       </c>
       <c r="B46">
-        <v>0.6395937204360962</v>
+        <v>1.551552772521973</v>
       </c>
       <c r="C46">
-        <v>4.714669704437256</v>
+        <v>0.424767017364502</v>
       </c>
       <c r="D46">
-        <v>1.163462042808533</v>
+        <v>4.866737365722656</v>
       </c>
       <c r="E46">
-        <v>0.4248944520950317</v>
+        <v>0.4233986735343933</v>
       </c>
       <c r="F46">
-        <v>0.5023835301399231</v>
+        <v>0.3216464519500732</v>
       </c>
       <c r="G46">
-        <v>0.4068045020103455</v>
+        <v>0.7868712544441223</v>
       </c>
       <c r="H46" t="s">
         <v>11</v>
       </c>
       <c r="I46">
-        <v>4.714669704437256</v>
+        <v>4.866737365722656</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B47">
-        <v>4.01276683807373</v>
+        <v>0.4189424514770508</v>
       </c>
       <c r="C47">
-        <v>0.7633211612701416</v>
+        <v>4.849438190460205</v>
       </c>
       <c r="D47">
-        <v>4.614940643310547</v>
+        <v>2.387334585189819</v>
       </c>
       <c r="E47">
-        <v>0.7574900984764099</v>
+        <v>0.3117768168449402</v>
       </c>
       <c r="F47">
-        <v>0.7204834818840027</v>
+        <v>0.4413956999778748</v>
       </c>
       <c r="G47">
-        <v>0.5914685130119324</v>
+        <v>0.4289876520633698</v>
       </c>
       <c r="H47" t="s">
         <v>10</v>
       </c>
       <c r="I47">
-        <v>4.614940643310547</v>
+        <v>4.849438190460205</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B48">
-        <v>0.4454178512096405</v>
+        <v>3.781533241271973</v>
       </c>
       <c r="C48">
-        <v>0.6496652960777283</v>
+        <v>0.4802358448505402</v>
       </c>
       <c r="D48">
-        <v>4.502804279327393</v>
+        <v>4.847046852111816</v>
       </c>
       <c r="E48">
-        <v>0.2845769822597504</v>
+        <v>0.4902788400650024</v>
       </c>
       <c r="F48">
-        <v>0.38226318359375</v>
+        <v>0.3585575222969055</v>
       </c>
       <c r="G48">
-        <v>0.7945255041122437</v>
+        <v>0.4632228016853333</v>
       </c>
       <c r="H48" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I48">
-        <v>4.502804279327393</v>
+        <v>4.847046852111816</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B49">
-        <v>4.500415802001953</v>
+        <v>4.83841609954834</v>
       </c>
       <c r="C49">
-        <v>0.5569881796836853</v>
+        <v>0.5888074040412903</v>
       </c>
       <c r="D49">
-        <v>4.179859161376953</v>
+        <v>2.668758153915405</v>
       </c>
       <c r="E49">
-        <v>0.5264094471931458</v>
+        <v>0.628690242767334</v>
       </c>
       <c r="F49">
-        <v>0.4748590886592865</v>
+        <v>0.4501321613788605</v>
       </c>
       <c r="G49">
-        <v>0.39176145195961</v>
+        <v>0.7621973752975464</v>
       </c>
       <c r="H49" t="s">
         <v>9</v>
       </c>
       <c r="I49">
-        <v>4.500415802001953</v>
+        <v>4.83841609954834</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B50">
-        <v>0.5741632580757141</v>
+        <v>0.4481925368309021</v>
       </c>
       <c r="C50">
-        <v>0.2683936953544617</v>
+        <v>0.4282205700874329</v>
       </c>
       <c r="D50">
-        <v>4.430737018585205</v>
+        <v>4.790715217590332</v>
       </c>
       <c r="E50">
-        <v>0.3272684216499329</v>
+        <v>0.3502523899078369</v>
       </c>
       <c r="F50">
-        <v>0.226508617401123</v>
+        <v>0.364632785320282</v>
       </c>
       <c r="G50">
-        <v>0.7038629055023193</v>
+        <v>0.5897634625434875</v>
       </c>
       <c r="H50" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I50">
-        <v>4.430737018585205</v>
+        <v>4.790715217590332</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B51">
-        <v>1.305639743804932</v>
+        <v>0.9914477467536926</v>
       </c>
       <c r="C51">
-        <v>4.369619846343994</v>
+        <v>0.4672659039497375</v>
       </c>
       <c r="D51">
-        <v>0.7050962448120117</v>
+        <v>4.749058246612549</v>
       </c>
       <c r="E51">
-        <v>0.3916561901569366</v>
+        <v>0.5011036992073059</v>
       </c>
       <c r="F51">
-        <v>0.5394195914268494</v>
+        <v>0.4619736969470978</v>
       </c>
       <c r="G51">
-        <v>0.3490701615810394</v>
+        <v>0.7746975421905518</v>
       </c>
       <c r="H51" t="s">
         <v>11</v>
       </c>
       <c r="I51">
-        <v>4.369619846343994</v>
+        <v>4.749058246612549</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B52">
-        <v>0.6664578914642334</v>
+        <v>0.893136739730835</v>
       </c>
       <c r="C52">
-        <v>0.2978371977806091</v>
+        <v>4.733603000640869</v>
       </c>
       <c r="D52">
-        <v>4.332044124603271</v>
+        <v>0.901543140411377</v>
       </c>
       <c r="E52">
-        <v>0.4753522574901581</v>
+        <v>0.4000642597675323</v>
       </c>
       <c r="F52">
-        <v>0.2598100900650024</v>
+        <v>0.6755520105361938</v>
       </c>
       <c r="G52">
-        <v>0.6294780969619751</v>
+        <v>0.3203251361846924</v>
       </c>
       <c r="H52" t="s">
         <v>10</v>
       </c>
       <c r="I52">
-        <v>4.332044124603271</v>
+        <v>4.733603000640869</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1926,463 +1926,463 @@
         <v>5</v>
       </c>
       <c r="B53">
-        <v>1.355974316596985</v>
+        <v>0.7053219676017761</v>
       </c>
       <c r="C53">
-        <v>4.268353939056396</v>
+        <v>4.731320381164551</v>
       </c>
       <c r="D53">
-        <v>1.982340812683105</v>
+        <v>0.8667781352996826</v>
       </c>
       <c r="E53">
-        <v>0.5961111783981323</v>
+        <v>0.5166423916816711</v>
       </c>
       <c r="F53">
-        <v>0.4303293526172638</v>
+        <v>0.4439172148704529</v>
       </c>
       <c r="G53">
-        <v>0.4786726534366608</v>
+        <v>0.3291881680488586</v>
       </c>
       <c r="H53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I53">
-        <v>4.268353939056396</v>
+        <v>4.731320381164551</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B54">
-        <v>0.6040122509002686</v>
+        <v>0.4563984572887421</v>
       </c>
       <c r="C54">
-        <v>4.232094287872314</v>
+        <v>0.3124713003635406</v>
       </c>
       <c r="D54">
-        <v>1.019957304000854</v>
+        <v>4.699315071105957</v>
       </c>
       <c r="E54">
-        <v>0.3886113464832306</v>
+        <v>0.3745470643043518</v>
       </c>
       <c r="F54">
-        <v>0.5056653618812561</v>
+        <v>0.2670880556106567</v>
       </c>
       <c r="G54">
-        <v>0.5104163885116577</v>
+        <v>0.6038521528244019</v>
       </c>
       <c r="H54" t="s">
         <v>11</v>
       </c>
       <c r="I54">
-        <v>4.232094287872314</v>
+        <v>4.699315071105957</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B55">
-        <v>0.580802857875824</v>
+        <v>0.8445910215377808</v>
       </c>
       <c r="C55">
-        <v>0.2405484765768051</v>
+        <v>0.4666413068771362</v>
       </c>
       <c r="D55">
-        <v>4.226453304290771</v>
+        <v>4.630508422851562</v>
       </c>
       <c r="E55">
-        <v>0.413757711648941</v>
+        <v>0.5383734703063965</v>
       </c>
       <c r="F55">
-        <v>0.3130834102630615</v>
+        <v>0.3988664448261261</v>
       </c>
       <c r="G55">
-        <v>0.5770449042320251</v>
+        <v>0.7169215679168701</v>
       </c>
       <c r="H55" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I55">
-        <v>4.226453304290771</v>
+        <v>4.630508422851562</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B56">
-        <v>1.409974813461304</v>
+        <v>4.539608955383301</v>
       </c>
       <c r="C56">
-        <v>0.3102516233921051</v>
+        <v>0.3935971260070801</v>
       </c>
       <c r="D56">
-        <v>4.214303493499756</v>
+        <v>1.139860033988953</v>
       </c>
       <c r="E56">
-        <v>0.4725889563560486</v>
+        <v>0.5297501087188721</v>
       </c>
       <c r="F56">
-        <v>0.2924222946166992</v>
+        <v>0.2938706278800964</v>
       </c>
       <c r="G56">
-        <v>0.792801558971405</v>
+        <v>0.5123305320739746</v>
       </c>
       <c r="H56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I56">
-        <v>4.214303493499756</v>
+        <v>4.539608955383301</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B57">
-        <v>0.9113236665725708</v>
+        <v>0.8324960470199585</v>
       </c>
       <c r="C57">
-        <v>0.2839363515377045</v>
+        <v>0.3498931527137756</v>
       </c>
       <c r="D57">
-        <v>4.210516929626465</v>
+        <v>4.51889705657959</v>
       </c>
       <c r="E57">
-        <v>0.2400173991918564</v>
+        <v>0.4642780721187592</v>
       </c>
       <c r="F57">
-        <v>0.3110118210315704</v>
+        <v>0.2907047867774963</v>
       </c>
       <c r="G57">
-        <v>0.4633802473545074</v>
+        <v>0.7341726422309875</v>
       </c>
       <c r="H57" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I57">
-        <v>4.210516929626465</v>
+        <v>4.51889705657959</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B58">
-        <v>1.280049324035645</v>
+        <v>0.4642939865589142</v>
       </c>
       <c r="C58">
-        <v>0.4687378704547882</v>
+        <v>4.406211376190186</v>
       </c>
       <c r="D58">
-        <v>4.209689617156982</v>
+        <v>0.8177953362464905</v>
       </c>
       <c r="E58">
-        <v>0.4944873452186584</v>
+        <v>0.3232595920562744</v>
       </c>
       <c r="F58">
-        <v>0.4602119922637939</v>
+        <v>0.4519906342029572</v>
       </c>
       <c r="G58">
-        <v>0.48182013630867</v>
+        <v>0.4266552031040192</v>
       </c>
       <c r="H58" t="s">
         <v>10</v>
       </c>
       <c r="I58">
-        <v>4.209689617156982</v>
+        <v>4.406211376190186</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B59">
-        <v>4.18530797958374</v>
+        <v>0.4880725741386414</v>
       </c>
       <c r="C59">
-        <v>0.7246070504188538</v>
+        <v>0.2735193967819214</v>
       </c>
       <c r="D59">
-        <v>0.3946442008018494</v>
+        <v>4.275888442993164</v>
       </c>
       <c r="E59">
-        <v>0.7900606989860535</v>
+        <v>0.3117102086544037</v>
       </c>
       <c r="F59">
-        <v>0.6767404675483704</v>
+        <v>0.2135924100875854</v>
       </c>
       <c r="G59">
-        <v>0.2838813364505768</v>
+        <v>0.6510772705078125</v>
       </c>
       <c r="H59" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I59">
-        <v>4.18530797958374</v>
+        <v>4.275888442993164</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B60">
-        <v>0.6062703728675842</v>
+        <v>4.156090259552002</v>
       </c>
       <c r="C60">
-        <v>0.3422911763191223</v>
+        <v>0.5319427847862244</v>
       </c>
       <c r="D60">
-        <v>4.174132823944092</v>
+        <v>0.6890122294425964</v>
       </c>
       <c r="E60">
-        <v>0.3984362483024597</v>
+        <v>0.7994129657745361</v>
       </c>
       <c r="F60">
-        <v>0.3280433714389801</v>
+        <v>0.3971633613109589</v>
       </c>
       <c r="G60">
-        <v>0.3193092346191406</v>
+        <v>0.2717465758323669</v>
       </c>
       <c r="H60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I60">
-        <v>4.174132823944092</v>
+        <v>4.156090259552002</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B61">
-        <v>0.3459592759609222</v>
+        <v>0.7100207209587097</v>
       </c>
       <c r="C61">
-        <v>4.143638134002686</v>
+        <v>4.119095802307129</v>
       </c>
       <c r="D61">
-        <v>1.082437753677368</v>
+        <v>1.88921594619751</v>
       </c>
       <c r="E61">
-        <v>0.2388529628515244</v>
+        <v>0.51664137840271</v>
       </c>
       <c r="F61">
-        <v>0.4013699889183044</v>
+        <v>0.4965206980705261</v>
       </c>
       <c r="G61">
-        <v>0.4284962713718414</v>
+        <v>0.5026926398277283</v>
       </c>
       <c r="H61" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I61">
-        <v>4.143638134002686</v>
+        <v>4.119095802307129</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B62">
-        <v>4.112292289733887</v>
+        <v>1.890835881233215</v>
       </c>
       <c r="C62">
-        <v>2.036388397216797</v>
+        <v>0.5649985671043396</v>
       </c>
       <c r="D62">
-        <v>3.237614870071411</v>
+        <v>4.113772869110107</v>
       </c>
       <c r="E62">
-        <v>0.3712125718593597</v>
+        <v>0.3650553524494171</v>
       </c>
       <c r="F62">
-        <v>0.4504758417606354</v>
+        <v>0.4829383492469788</v>
       </c>
       <c r="G62">
-        <v>0.4522309005260468</v>
+        <v>0.559736430644989</v>
       </c>
       <c r="H62" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I62">
-        <v>4.112292289733887</v>
+        <v>4.113772869110107</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B63">
-        <v>3.367501974105835</v>
+        <v>0.9917532205581665</v>
       </c>
       <c r="C63">
-        <v>0.5562509894371033</v>
+        <v>0.3003247082233429</v>
       </c>
       <c r="D63">
-        <v>3.883129119873047</v>
+        <v>4.09610652923584</v>
       </c>
       <c r="E63">
-        <v>0.4338265061378479</v>
+        <v>0.7896836996078491</v>
       </c>
       <c r="F63">
-        <v>0.4865312278270721</v>
+        <v>0.2510789334774017</v>
       </c>
       <c r="G63">
-        <v>0.5591688752174377</v>
+        <v>0.3769412636756897</v>
       </c>
       <c r="H63" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I63">
-        <v>3.883129119873047</v>
+        <v>4.09610652923584</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B64">
-        <v>0.5188497304916382</v>
+        <v>1.031310439109802</v>
       </c>
       <c r="C64">
-        <v>3.879443407058716</v>
+        <v>0.5996295809745789</v>
       </c>
       <c r="D64">
-        <v>3.853436708450317</v>
+        <v>4.039260864257812</v>
       </c>
       <c r="E64">
-        <v>0.3600914776325226</v>
+        <v>0.4610050320625305</v>
       </c>
       <c r="F64">
-        <v>0.4543478488922119</v>
+        <v>0.446944385766983</v>
       </c>
       <c r="G64">
-        <v>0.5509883761405945</v>
+        <v>0.5864284634590149</v>
       </c>
       <c r="H64" t="s">
         <v>11</v>
       </c>
       <c r="I64">
-        <v>3.879443407058716</v>
+        <v>4.039260864257812</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B65">
-        <v>0.7998548746109009</v>
+        <v>0.8226422071456909</v>
       </c>
       <c r="C65">
-        <v>2.511055469512939</v>
+        <v>0.3340491056442261</v>
       </c>
       <c r="D65">
-        <v>3.87824010848999</v>
+        <v>3.981106281280518</v>
       </c>
       <c r="E65">
-        <v>0.591956615447998</v>
+        <v>0.4232445061206818</v>
       </c>
       <c r="F65">
-        <v>0.3666545152664185</v>
+        <v>0.3274177312850952</v>
       </c>
       <c r="G65">
-        <v>0.4530238807201385</v>
+        <v>0.6860789060592651</v>
       </c>
       <c r="H65" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I65">
-        <v>3.87824010848999</v>
+        <v>3.981106281280518</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B66">
-        <v>0.5584484338760376</v>
+        <v>0.5980485677719116</v>
       </c>
       <c r="C66">
-        <v>0.6152045130729675</v>
+        <v>0.3933755159378052</v>
       </c>
       <c r="D66">
-        <v>3.869146585464478</v>
+        <v>3.907949447631836</v>
       </c>
       <c r="E66">
-        <v>0.272204726934433</v>
+        <v>0.4351656436920166</v>
       </c>
       <c r="F66">
-        <v>0.2968957722187042</v>
+        <v>0.3556659519672394</v>
       </c>
       <c r="G66">
-        <v>0.4179515242576599</v>
+        <v>0.4780019223690033</v>
       </c>
       <c r="H66" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I66">
-        <v>3.869146585464478</v>
+        <v>3.907949447631836</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B67">
-        <v>0.5153672695159912</v>
+        <v>0.4906657636165619</v>
       </c>
       <c r="C67">
-        <v>1.450673818588257</v>
+        <v>1.144004225730896</v>
       </c>
       <c r="D67">
-        <v>3.855592012405396</v>
+        <v>3.895614147186279</v>
       </c>
       <c r="E67">
-        <v>0.3682010769844055</v>
+        <v>0.3932327628135681</v>
       </c>
       <c r="F67">
-        <v>0.6729082465171814</v>
+        <v>0.2939709722995758</v>
       </c>
       <c r="G67">
-        <v>0.4717908799648285</v>
+        <v>0.7723187208175659</v>
       </c>
       <c r="H67" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I67">
-        <v>3.855592012405396</v>
+        <v>3.895614147186279</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B68">
-        <v>1.044631600379944</v>
+        <v>0.5013094544410706</v>
       </c>
       <c r="C68">
-        <v>0.1993452161550522</v>
+        <v>0.3587182462215424</v>
       </c>
       <c r="D68">
-        <v>3.842098712921143</v>
+        <v>3.822210550308228</v>
       </c>
       <c r="E68">
-        <v>0.7362015843391418</v>
+        <v>0.3136215209960938</v>
       </c>
       <c r="F68">
-        <v>0.2277786582708359</v>
+        <v>0.3054141700267792</v>
       </c>
       <c r="G68">
-        <v>0.5415493249893188</v>
+        <v>0.416873037815094</v>
       </c>
       <c r="H68" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I68">
-        <v>3.842098712921143</v>
+        <v>3.822210550308228</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2390,231 +2390,231 @@
         <v>3</v>
       </c>
       <c r="B69">
-        <v>0.4497923851013184</v>
+        <v>1.505558609962463</v>
       </c>
       <c r="C69">
-        <v>3.836776494979858</v>
+        <v>3.149876356124878</v>
       </c>
       <c r="D69">
-        <v>1.168477535247803</v>
+        <v>3.806783437728882</v>
       </c>
       <c r="E69">
-        <v>0.320427268743515</v>
+        <v>0.5935945510864258</v>
       </c>
       <c r="F69">
-        <v>0.585633397102356</v>
+        <v>0.331248939037323</v>
       </c>
       <c r="G69">
-        <v>0.4303281009197235</v>
+        <v>0.6093037724494934</v>
       </c>
       <c r="H69" t="s">
         <v>11</v>
       </c>
       <c r="I69">
-        <v>3.836776494979858</v>
+        <v>3.806783437728882</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B70">
-        <v>0.582064151763916</v>
+        <v>0.6109322905540466</v>
       </c>
       <c r="C70">
-        <v>0.6740126609802246</v>
+        <v>0.2279471457004547</v>
       </c>
       <c r="D70">
-        <v>3.787899971008301</v>
+        <v>3.757925510406494</v>
       </c>
       <c r="E70">
-        <v>0.380597710609436</v>
+        <v>0.3834899663925171</v>
       </c>
       <c r="F70">
-        <v>0.3769183754920959</v>
+        <v>0.2991949319839478</v>
       </c>
       <c r="G70">
-        <v>0.681069552898407</v>
+        <v>0.5106891989707947</v>
       </c>
       <c r="H70" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I70">
-        <v>3.787899971008301</v>
+        <v>3.757925510406494</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B71">
-        <v>0.6732867956161499</v>
+        <v>3.727618932723999</v>
       </c>
       <c r="C71">
-        <v>0.493439108133316</v>
+        <v>2.118308305740356</v>
       </c>
       <c r="D71">
-        <v>3.719396352767944</v>
+        <v>0.72627192735672</v>
       </c>
       <c r="E71">
-        <v>0.4868099689483643</v>
+        <v>0.7994129657745361</v>
       </c>
       <c r="F71">
-        <v>0.415654718875885</v>
+        <v>0.7267957329750061</v>
       </c>
       <c r="G71">
-        <v>0.6389650702476501</v>
+        <v>0.5224327445030212</v>
       </c>
       <c r="H71" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I71">
-        <v>3.719396352767944</v>
+        <v>3.727618932723999</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B72">
-        <v>0.5916579365730286</v>
+        <v>3.720351219177246</v>
       </c>
       <c r="C72">
-        <v>0.1805351376533508</v>
+        <v>0.7040278315544128</v>
       </c>
       <c r="D72">
-        <v>3.696828126907349</v>
+        <v>0.5345684289932251</v>
       </c>
       <c r="E72">
-        <v>0.4547415375709534</v>
+        <v>0.7994129657745361</v>
       </c>
       <c r="F72">
-        <v>0.2643669247627258</v>
+        <v>0.3584563136100769</v>
       </c>
       <c r="G72">
-        <v>0.5296776294708252</v>
+        <v>0.3845337331295013</v>
       </c>
       <c r="H72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I72">
-        <v>3.696828126907349</v>
+        <v>3.720351219177246</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B73">
-        <v>0.7457153797149658</v>
+        <v>0.5700875520706177</v>
       </c>
       <c r="C73">
-        <v>0.3995901346206665</v>
+        <v>2.832683324813843</v>
       </c>
       <c r="D73">
-        <v>3.674150228500366</v>
+        <v>3.702699899673462</v>
       </c>
       <c r="E73">
-        <v>0.4353805780410767</v>
+        <v>0.4360840618610382</v>
       </c>
       <c r="F73">
-        <v>0.2213827520608902</v>
+        <v>0.4802608788013458</v>
       </c>
       <c r="G73">
-        <v>0.5500881671905518</v>
+        <v>0.5983478426933289</v>
       </c>
       <c r="H73" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I73">
-        <v>3.674150228500366</v>
+        <v>3.702699899673462</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B74">
-        <v>0.5590777993202209</v>
+        <v>3.656884670257568</v>
       </c>
       <c r="C74">
-        <v>1.424061179161072</v>
+        <v>0.1667796671390533</v>
       </c>
       <c r="D74">
-        <v>3.626932859420776</v>
+        <v>0.6920757293701172</v>
       </c>
       <c r="E74">
-        <v>0.3994297981262207</v>
+        <v>0.7994129657745361</v>
       </c>
       <c r="F74">
-        <v>0.4005314111709595</v>
+        <v>0.2135924100875854</v>
       </c>
       <c r="G74">
-        <v>0.4494007229804993</v>
+        <v>0.4978342056274414</v>
       </c>
       <c r="H74" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I74">
-        <v>3.626932859420776</v>
+        <v>3.656884670257568</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B75">
-        <v>1.000615477561951</v>
+        <v>3.630910396575928</v>
       </c>
       <c r="C75">
-        <v>0.4275351464748383</v>
+        <v>0.5896835923194885</v>
       </c>
       <c r="D75">
-        <v>3.609516143798828</v>
+        <v>1.076756715774536</v>
       </c>
       <c r="E75">
-        <v>0.4393072128295898</v>
+        <v>0.7046433091163635</v>
       </c>
       <c r="F75">
-        <v>0.2486212402582169</v>
+        <v>0.4311937987804413</v>
       </c>
       <c r="G75">
-        <v>0.438384622335434</v>
+        <v>0.3982928395271301</v>
       </c>
       <c r="H75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I75">
-        <v>3.609516143798828</v>
+        <v>3.630910396575928</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B76">
-        <v>0.3336067497730255</v>
+        <v>0.3396424055099487</v>
       </c>
       <c r="C76">
-        <v>0.4892699420452118</v>
+        <v>0.8260922431945801</v>
       </c>
       <c r="D76">
-        <v>3.602411270141602</v>
+        <v>3.539930105209351</v>
       </c>
       <c r="E76">
-        <v>0.2409688085317612</v>
+        <v>0.2347748875617981</v>
       </c>
       <c r="F76">
-        <v>0.5706766247749329</v>
+        <v>0.5209513306617737</v>
       </c>
       <c r="G76">
-        <v>0.5308374762535095</v>
+        <v>0.4532313048839569</v>
       </c>
       <c r="H76" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I76">
-        <v>3.602411270141602</v>
+        <v>3.539930105209351</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -2622,202 +2622,202 @@
         <v>4</v>
       </c>
       <c r="B77">
-        <v>3.571057796478271</v>
+        <v>0.6625139713287354</v>
       </c>
       <c r="C77">
-        <v>0.1704869121313095</v>
+        <v>0.4019263982772827</v>
       </c>
       <c r="D77">
-        <v>0.5966870784759521</v>
+        <v>3.535719156265259</v>
       </c>
       <c r="E77">
-        <v>0.7817679643630981</v>
+        <v>0.3931671380996704</v>
       </c>
       <c r="F77">
-        <v>0.2187499701976776</v>
+        <v>0.3310569226741791</v>
       </c>
       <c r="G77">
-        <v>0.4292178452014923</v>
+        <v>0.482308030128479</v>
       </c>
       <c r="H77" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I77">
-        <v>3.571057796478271</v>
+        <v>3.535719156265259</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B78">
-        <v>3.492010116577148</v>
+        <v>0.6960919499397278</v>
       </c>
       <c r="C78">
-        <v>0.2414712011814117</v>
+        <v>3.492576360702515</v>
       </c>
       <c r="D78">
-        <v>0.9645367860794067</v>
+        <v>0.9642453789710999</v>
       </c>
       <c r="E78">
-        <v>0.7896054983139038</v>
+        <v>0.4249018728733063</v>
       </c>
       <c r="F78">
-        <v>0.2187499701976776</v>
+        <v>0.2901385426521301</v>
       </c>
       <c r="G78">
-        <v>0.3415709733963013</v>
+        <v>0.5534840226173401</v>
       </c>
       <c r="H78" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I78">
-        <v>3.492010116577148</v>
+        <v>3.492576360702515</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B79">
-        <v>3.436897754669189</v>
+        <v>0.3581470549106598</v>
       </c>
       <c r="C79">
-        <v>0.3438328206539154</v>
+        <v>0.3720684051513672</v>
       </c>
       <c r="D79">
-        <v>0.9212982058525085</v>
+        <v>3.39698052406311</v>
       </c>
       <c r="E79">
-        <v>0.4020107388496399</v>
+        <v>0.2873785197734833</v>
       </c>
       <c r="F79">
-        <v>0.3035051822662354</v>
+        <v>0.2688964903354645</v>
       </c>
       <c r="G79">
-        <v>0.439231812953949</v>
+        <v>0.7568113803863525</v>
       </c>
       <c r="H79" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I79">
-        <v>3.436897754669189</v>
+        <v>3.39698052406311</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B80">
-        <v>0.5387656688690186</v>
+        <v>0.4587962925434113</v>
       </c>
       <c r="C80">
-        <v>0.4251333475112915</v>
+        <v>0.3751829564571381</v>
       </c>
       <c r="D80">
-        <v>3.434826850891113</v>
+        <v>3.393002033233643</v>
       </c>
       <c r="E80">
-        <v>0.4787610471248627</v>
+        <v>0.3369752466678619</v>
       </c>
       <c r="F80">
-        <v>0.3960905969142914</v>
+        <v>0.3602729141712189</v>
       </c>
       <c r="G80">
-        <v>0.7043770551681519</v>
+        <v>0.5477235913276672</v>
       </c>
       <c r="H80" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I80">
-        <v>3.434826850891113</v>
+        <v>3.393002033233643</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B81">
-        <v>3.411182641983032</v>
+        <v>2.100971221923828</v>
       </c>
       <c r="C81">
-        <v>0.3434814214706421</v>
+        <v>0.3449104726314545</v>
       </c>
       <c r="D81">
-        <v>0.4742518067359924</v>
+        <v>3.375360012054443</v>
       </c>
       <c r="E81">
-        <v>0.70946204662323</v>
+        <v>0.517899215221405</v>
       </c>
       <c r="F81">
-        <v>0.2314237654209137</v>
+        <v>0.3093777000904083</v>
       </c>
       <c r="G81">
-        <v>0.2187835574150085</v>
+        <v>0.6484608054161072</v>
       </c>
       <c r="H81" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I81">
-        <v>3.411182641983032</v>
+        <v>3.375360012054443</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B82">
-        <v>0.4360147416591644</v>
+        <v>3.370040416717529</v>
       </c>
       <c r="C82">
-        <v>0.5494910478591919</v>
+        <v>1.030431509017944</v>
       </c>
       <c r="D82">
-        <v>3.348251342773438</v>
+        <v>1.069309830665588</v>
       </c>
       <c r="E82">
-        <v>0.3783649802207947</v>
+        <v>0.7994129657745361</v>
       </c>
       <c r="F82">
-        <v>0.3679676353931427</v>
+        <v>0.7693489789962769</v>
       </c>
       <c r="G82">
-        <v>0.5356680750846863</v>
+        <v>0.5488765835762024</v>
       </c>
       <c r="H82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I82">
-        <v>3.348251342773438</v>
+        <v>3.370040416717529</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B83">
-        <v>0.8494998812675476</v>
+        <v>0.9775951504707336</v>
       </c>
       <c r="C83">
-        <v>3.248117446899414</v>
+        <v>0.4166362285614014</v>
       </c>
       <c r="D83">
-        <v>2.225080728530884</v>
+        <v>3.361559867858887</v>
       </c>
       <c r="E83">
-        <v>0.6909928321838379</v>
+        <v>0.5336503386497498</v>
       </c>
       <c r="F83">
-        <v>0.4752231240272522</v>
+        <v>0.2706896066665649</v>
       </c>
       <c r="G83">
-        <v>0.703268826007843</v>
+        <v>0.6126221418380737</v>
       </c>
       <c r="H83" t="s">
         <v>11</v>
       </c>
       <c r="I83">
-        <v>3.248117446899414</v>
+        <v>3.361559867858887</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -2825,202 +2825,202 @@
         <v>2</v>
       </c>
       <c r="B84">
-        <v>0.8190135359764099</v>
+        <v>1.054706931114197</v>
       </c>
       <c r="C84">
-        <v>0.3441135287284851</v>
+        <v>3.35699725151062</v>
       </c>
       <c r="D84">
-        <v>3.215967416763306</v>
+        <v>0.8167909383773804</v>
       </c>
       <c r="E84">
-        <v>0.5348133444786072</v>
+        <v>0.4015385508537292</v>
       </c>
       <c r="F84">
-        <v>0.3804852366447449</v>
+        <v>0.4813903868198395</v>
       </c>
       <c r="G84">
-        <v>0.55064457654953</v>
+        <v>0.3193217217922211</v>
       </c>
       <c r="H84" t="s">
         <v>10</v>
       </c>
       <c r="I84">
-        <v>3.215967416763306</v>
+        <v>3.35699725151062</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B85">
-        <v>0.8202193975448608</v>
+        <v>0.7292965054512024</v>
       </c>
       <c r="C85">
-        <v>0.4633361101150513</v>
+        <v>3.327057361602783</v>
       </c>
       <c r="D85">
-        <v>3.121118783950806</v>
+        <v>0.9167100787162781</v>
       </c>
       <c r="E85">
-        <v>0.4253511130809784</v>
+        <v>0.530667245388031</v>
       </c>
       <c r="F85">
-        <v>0.371159553527832</v>
+        <v>0.5640783905982971</v>
       </c>
       <c r="G85">
-        <v>0.3667866289615631</v>
+        <v>0.4521487951278687</v>
       </c>
       <c r="H85" t="s">
         <v>10</v>
       </c>
       <c r="I85">
-        <v>3.121118783950806</v>
+        <v>3.327057361602783</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="B86">
-        <v>0.6299841403961182</v>
+        <v>0.5809359550476074</v>
       </c>
       <c r="C86">
-        <v>0.436733603477478</v>
+        <v>3.196850776672363</v>
       </c>
       <c r="D86">
-        <v>3.043490409851074</v>
+        <v>1.499341726303101</v>
       </c>
       <c r="E86">
-        <v>0.4819014966487885</v>
+        <v>0.4227137863636017</v>
       </c>
       <c r="F86">
-        <v>0.3729179501533508</v>
+        <v>0.3634963035583496</v>
       </c>
       <c r="G86">
-        <v>0.3363138735294342</v>
+        <v>0.5602391362190247</v>
       </c>
       <c r="H86" t="s">
         <v>10</v>
       </c>
       <c r="I86">
-        <v>3.043490409851074</v>
+        <v>3.196850776672363</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B87">
-        <v>0.6118919253349304</v>
+        <v>3.164202928543091</v>
       </c>
       <c r="C87">
-        <v>1.046817541122437</v>
+        <v>0.405200332403183</v>
       </c>
       <c r="D87">
-        <v>3.034385442733765</v>
+        <v>1.455923080444336</v>
       </c>
       <c r="E87">
-        <v>0.2363758981227875</v>
+        <v>0.3911035656929016</v>
       </c>
       <c r="F87">
-        <v>0.3723730146884918</v>
+        <v>0.3463491499423981</v>
       </c>
       <c r="G87">
-        <v>0.4756392538547516</v>
+        <v>0.583274781703949</v>
       </c>
       <c r="H87" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I87">
-        <v>3.034385442733765</v>
+        <v>3.164202928543091</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B88">
-        <v>0.4639895558357239</v>
+        <v>0.6109759211540222</v>
       </c>
       <c r="C88">
-        <v>0.8950289487838745</v>
+        <v>0.2865130007266998</v>
       </c>
       <c r="D88">
-        <v>3.007312297821045</v>
+        <v>3.148149728775024</v>
       </c>
       <c r="E88">
-        <v>0.4092554152011871</v>
+        <v>0.3739249408245087</v>
       </c>
       <c r="F88">
-        <v>0.6800346970558167</v>
+        <v>0.2628198862075806</v>
       </c>
       <c r="G88">
-        <v>0.4359100759029388</v>
+        <v>0.6936537623405457</v>
       </c>
       <c r="H88" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I88">
-        <v>3.007312297821045</v>
+        <v>3.148149728775024</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B89">
-        <v>2.992449045181274</v>
+        <v>3.13843560218811</v>
       </c>
       <c r="C89">
-        <v>0.2939099669456482</v>
+        <v>0.3756946325302124</v>
       </c>
       <c r="D89">
-        <v>0.4744851589202881</v>
+        <v>1.149006962776184</v>
       </c>
       <c r="E89">
-        <v>0.6522709727287292</v>
+        <v>0.6043991446495056</v>
       </c>
       <c r="F89">
-        <v>0.2448031902313232</v>
+        <v>0.3199065923690796</v>
       </c>
       <c r="G89">
-        <v>0.3413137197494507</v>
+        <v>0.5613760948181152</v>
       </c>
       <c r="H89" t="s">
         <v>9</v>
       </c>
       <c r="I89">
-        <v>2.992449045181274</v>
+        <v>3.13843560218811</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B90">
-        <v>2.992449045181274</v>
+        <v>0.5365393757820129</v>
       </c>
       <c r="C90">
-        <v>0.317261129617691</v>
+        <v>0.8373998999595642</v>
       </c>
       <c r="D90">
-        <v>1.405728101730347</v>
+        <v>3.105318307876587</v>
       </c>
       <c r="E90">
-        <v>0.6522709727287292</v>
+        <v>0.3947248756885529</v>
       </c>
       <c r="F90">
-        <v>0.3873101472854614</v>
+        <v>0.5670300722122192</v>
       </c>
       <c r="G90">
-        <v>0.7204980254173279</v>
+        <v>0.4784827828407288</v>
       </c>
       <c r="H90" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I90">
-        <v>2.992449045181274</v>
+        <v>3.105318307876587</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3028,57 +3028,57 @@
         <v>2</v>
       </c>
       <c r="B91">
-        <v>0.5214720964431763</v>
+        <v>3.095589399337769</v>
       </c>
       <c r="C91">
-        <v>2.979122161865234</v>
+        <v>0.3390181958675385</v>
       </c>
       <c r="D91">
-        <v>1.619511961936951</v>
+        <v>0.6993029713630676</v>
       </c>
       <c r="E91">
-        <v>0.3714911043643951</v>
+        <v>0.6007546782493591</v>
       </c>
       <c r="F91">
-        <v>0.3593218624591827</v>
+        <v>0.4052734971046448</v>
       </c>
       <c r="G91">
-        <v>0.438157320022583</v>
+        <v>0.4540975689888</v>
       </c>
       <c r="H91" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I91">
-        <v>2.979122161865234</v>
+        <v>3.095589399337769</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B92">
-        <v>2.943866968154907</v>
+        <v>3.071769237518311</v>
       </c>
       <c r="C92">
-        <v>2.381513118743896</v>
+        <v>0.9807472825050354</v>
       </c>
       <c r="D92">
-        <v>0.9079650640487671</v>
+        <v>2.944495439529419</v>
       </c>
       <c r="E92">
-        <v>0.6522709727287292</v>
+        <v>0.4435325264930725</v>
       </c>
       <c r="F92">
-        <v>0.7612464427947998</v>
+        <v>0.7567992806434631</v>
       </c>
       <c r="G92">
-        <v>0.6531309485435486</v>
+        <v>0.5067654848098755</v>
       </c>
       <c r="H92" t="s">
         <v>9</v>
       </c>
       <c r="I92">
-        <v>2.943866968154907</v>
+        <v>3.071769237518311</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -3086,144 +3086,144 @@
         <v>2</v>
       </c>
       <c r="B93">
-        <v>0.9457775950431824</v>
+        <v>3.047333240509033</v>
       </c>
       <c r="C93">
-        <v>2.883020639419556</v>
+        <v>0.19334976375103</v>
       </c>
       <c r="D93">
-        <v>1.116384983062744</v>
+        <v>0.6415472030639648</v>
       </c>
       <c r="E93">
-        <v>0.4528072774410248</v>
+        <v>0.5913897156715393</v>
       </c>
       <c r="F93">
-        <v>0.4209674298763275</v>
+        <v>0.213011309504509</v>
       </c>
       <c r="G93">
-        <v>0.5802174806594849</v>
+        <v>0.2711325287818909</v>
       </c>
       <c r="H93" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I93">
-        <v>2.883020639419556</v>
+        <v>3.047333240509033</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B94">
-        <v>0.5562331080436707</v>
+        <v>3.031226396560669</v>
       </c>
       <c r="C94">
-        <v>0.6611424684524536</v>
+        <v>0.4728284478187561</v>
       </c>
       <c r="D94">
-        <v>2.880934953689575</v>
+        <v>0.8834133148193359</v>
       </c>
       <c r="E94">
-        <v>0.4064222872257233</v>
+        <v>0.4610541462898254</v>
       </c>
       <c r="F94">
-        <v>0.294289231300354</v>
+        <v>0.4634421169757843</v>
       </c>
       <c r="G94">
-        <v>0.4153705239295959</v>
+        <v>0.496905654668808</v>
       </c>
       <c r="H94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I94">
-        <v>2.880934953689575</v>
+        <v>3.031226396560669</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B95">
-        <v>1.014406442642212</v>
+        <v>0.5650938749313354</v>
       </c>
       <c r="C95">
-        <v>2.87935209274292</v>
+        <v>0.3066739439964294</v>
       </c>
       <c r="D95">
-        <v>0.5729262828826904</v>
+        <v>3.030506610870361</v>
       </c>
       <c r="E95">
-        <v>0.7149004936218262</v>
+        <v>0.3095986843109131</v>
       </c>
       <c r="F95">
-        <v>0.7476269602775574</v>
+        <v>0.2508777678012848</v>
       </c>
       <c r="G95">
-        <v>0.2828547358512878</v>
+        <v>0.4257056415081024</v>
       </c>
       <c r="H95" t="s">
         <v>11</v>
       </c>
       <c r="I95">
-        <v>2.87935209274292</v>
+        <v>3.030506610870361</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B96">
-        <v>1.804637670516968</v>
+        <v>2.998093128204346</v>
       </c>
       <c r="C96">
-        <v>0.8272866606712341</v>
+        <v>0.3528673350811005</v>
       </c>
       <c r="D96">
-        <v>2.852256536483765</v>
+        <v>1.58150577545166</v>
       </c>
       <c r="E96">
-        <v>0.6381067633628845</v>
+        <v>0.7994129657745361</v>
       </c>
       <c r="F96">
-        <v>0.3091905117034912</v>
+        <v>0.4519123136997223</v>
       </c>
       <c r="G96">
-        <v>0.5176571011543274</v>
+        <v>0.7511909604072571</v>
       </c>
       <c r="H96" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I96">
-        <v>2.852256536483765</v>
+        <v>2.998093128204346</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B97">
-        <v>2.842087745666504</v>
+        <v>2.96199631690979</v>
       </c>
       <c r="C97">
-        <v>0.2687933743000031</v>
+        <v>0.2655887007713318</v>
       </c>
       <c r="D97">
-        <v>1.252828359603882</v>
+        <v>0.9587277173995972</v>
       </c>
       <c r="E97">
-        <v>0.3324363529682159</v>
+        <v>0.7994129657745361</v>
       </c>
       <c r="F97">
-        <v>0.2483253479003906</v>
+        <v>0.2135924100875854</v>
       </c>
       <c r="G97">
-        <v>0.5564073324203491</v>
+        <v>0.4066411256790161</v>
       </c>
       <c r="H97" t="s">
         <v>9</v>
       </c>
       <c r="I97">
-        <v>2.842087745666504</v>
+        <v>2.96199631690979</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -3231,57 +3231,57 @@
         <v>3</v>
       </c>
       <c r="B98">
-        <v>2.840349435806274</v>
+        <v>0.7937278747558594</v>
       </c>
       <c r="C98">
-        <v>0.707105815410614</v>
+        <v>0.2560145258903503</v>
       </c>
       <c r="D98">
-        <v>0.6224014163017273</v>
+        <v>2.943710803985596</v>
       </c>
       <c r="E98">
-        <v>0.7900606989860535</v>
+        <v>0.4004085958003998</v>
       </c>
       <c r="F98">
-        <v>0.6401103138923645</v>
+        <v>0.2486229240894318</v>
       </c>
       <c r="G98">
-        <v>0.4477150738239288</v>
+        <v>0.3574491739273071</v>
       </c>
       <c r="H98" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I98">
-        <v>2.840349435806274</v>
+        <v>2.943710803985596</v>
       </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B99">
-        <v>2.840085983276367</v>
+        <v>0.5455041527748108</v>
       </c>
       <c r="C99">
-        <v>0.3279384970664978</v>
+        <v>0.1879736036062241</v>
       </c>
       <c r="D99">
-        <v>0.7872990965843201</v>
+        <v>2.927243947982788</v>
       </c>
       <c r="E99">
-        <v>0.7778476476669312</v>
+        <v>0.4300900399684906</v>
       </c>
       <c r="F99">
-        <v>0.3095730841159821</v>
+        <v>0.2131977826356888</v>
       </c>
       <c r="G99">
-        <v>0.4081725180149078</v>
+        <v>0.4129853546619415</v>
       </c>
       <c r="H99" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I99">
-        <v>2.840085983276367</v>
+        <v>2.927243947982788</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -3289,28 +3289,28 @@
         <v>2</v>
       </c>
       <c r="B100">
-        <v>2.592391014099121</v>
+        <v>0.4855437278747559</v>
       </c>
       <c r="C100">
-        <v>0.2667898833751678</v>
+        <v>0.5148630738258362</v>
       </c>
       <c r="D100">
-        <v>2.789860010147095</v>
+        <v>2.922348737716675</v>
       </c>
       <c r="E100">
-        <v>0.4781155586242676</v>
+        <v>0.40896075963974</v>
       </c>
       <c r="F100">
-        <v>0.3587712943553925</v>
+        <v>0.2567630410194397</v>
       </c>
       <c r="G100">
-        <v>0.4303486049175262</v>
+        <v>0.6547122597694397</v>
       </c>
       <c r="H100" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I100">
-        <v>2.789860010147095</v>
+        <v>2.922348737716675</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -3318,28 +3318,28 @@
         <v>4</v>
       </c>
       <c r="B101">
-        <v>1.114575505256653</v>
+        <v>1.072011470794678</v>
       </c>
       <c r="C101">
-        <v>2.780062437057495</v>
+        <v>0.257658064365387</v>
       </c>
       <c r="D101">
-        <v>0.9403793215751648</v>
+        <v>2.913803100585938</v>
       </c>
       <c r="E101">
-        <v>0.6707724928855896</v>
+        <v>0.2651011943817139</v>
       </c>
       <c r="F101">
-        <v>0.678011417388916</v>
+        <v>0.3340701460838318</v>
       </c>
       <c r="G101">
-        <v>0.5025174021720886</v>
+        <v>0.4336075484752655</v>
       </c>
       <c r="H101" t="s">
         <v>11</v>
       </c>
       <c r="I101">
-        <v>2.780062437057495</v>
+        <v>2.913803100585938</v>
       </c>
     </row>
   </sheetData>

</xml_diff>